<commit_message>
update timetable and fix syntax error
</commit_message>
<xml_diff>
--- a/assets/paris-saclay-l3-info.xlsx
+++ b/assets/paris-saclay-l3-info.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="86">
   <si>
     <r>
       <rPr>
@@ -38,7 +38,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">10/09/2020</t>
+      <t xml:space="preserve">11/09/2020</t>
     </r>
   </si>
   <si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t xml:space="preserve">15:45 17:45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13:30 15:30</t>
   </si>
   <si>
     <t xml:space="preserve">31/08/20</t>
@@ -373,6 +376,9 @@
     <t xml:space="preserve">21/09/20</t>
   </si>
   <si>
+    <t xml:space="preserve">* Les TD de Réseaux sont à 10h.</t>
+  </si>
+  <si>
     <t xml:space="preserve">TD GLA G1/D203</t>
   </si>
   <si>
@@ -402,15 +408,49 @@
 G1/D203</t>
   </si>
   <si>
-    <t xml:space="preserve">@[10:00 12:45]TD Réseaux
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">* </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">TD Réseaux
 G2/E105</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">TD GLA G2 D203</t>
   </si>
   <si>
-    <t xml:space="preserve">@[10:00 12:45]TD Réseaux
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">* </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">TD Réseaux
 G3/E212</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">28/09/20</t>
@@ -473,8 +513,25 @@
     <t xml:space="preserve">FERIE</t>
   </si>
   <si>
-    <t xml:space="preserve">@[10:00 12:45]TD Réseaux
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">* </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">TD Réseaux
 G2/B107</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">TP GLA G3 E204</t>
@@ -788,7 +845,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -899,10 +956,6 @@
     </xf>
     <xf numFmtId="164" fontId="13" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1040,8 +1093,8 @@
   </sheetPr>
   <dimension ref="A1:AG58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB8" activeCellId="0" sqref="AB8:AB10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y23" activeCellId="0" sqref="Y23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1268,7 +1321,7 @@
       </c>
       <c r="W4" s="8"/>
       <c r="X4" s="9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="Y4" s="9" t="s">
         <v>16</v>
@@ -1290,7 +1343,7 @@
     <row r="5" customFormat="false" ht="38.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2"/>
       <c r="B5" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -1302,7 +1355,7 @@
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
       <c r="L5" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M5" s="8"/>
       <c r="N5" s="7"/>
@@ -1362,7 +1415,7 @@
     <row r="7" customFormat="false" ht="78.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2"/>
       <c r="B7" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -1372,39 +1425,39 @@
       <c r="H7" s="13"/>
       <c r="I7" s="14"/>
       <c r="J7" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K7" s="8"/>
       <c r="L7" s="16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M7" s="16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N7" s="7"/>
       <c r="O7" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P7" s="8"/>
       <c r="Q7" s="8"/>
       <c r="R7" s="18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="S7" s="8"/>
       <c r="T7" s="7"/>
       <c r="U7" s="19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="V7" s="8"/>
       <c r="W7" s="20"/>
       <c r="X7" s="18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Y7" s="8"/>
       <c r="Z7" s="7"/>
       <c r="AA7" s="14"/>
       <c r="AB7" s="21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AC7" s="12"/>
       <c r="AD7" s="8"/>
@@ -1414,63 +1467,63 @@
     <row r="8" customFormat="false" ht="19.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2"/>
       <c r="B8" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="7"/>
       <c r="I8" s="23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K8" s="8"/>
       <c r="L8" s="16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M8" s="23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N8" s="7"/>
       <c r="O8" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P8" s="24" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q8" s="8"/>
       <c r="R8" s="18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="S8" s="25"/>
       <c r="T8" s="7"/>
       <c r="U8" s="19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="V8" s="8"/>
       <c r="W8" s="20"/>
       <c r="X8" s="26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Y8" s="22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Z8" s="7"/>
       <c r="AA8" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB8" s="28" t="s">
-        <v>26</v>
+        <v>37</v>
+      </c>
+      <c r="AB8" s="21" t="s">
+        <v>27</v>
       </c>
       <c r="AC8" s="20"/>
       <c r="AD8" s="27" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AE8" s="27"/>
       <c r="AF8" s="8"/>
@@ -1492,7 +1545,7 @@
       <c r="N9" s="7"/>
       <c r="O9" s="17"/>
       <c r="P9" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q9" s="8"/>
       <c r="R9" s="18"/>
@@ -1502,12 +1555,12 @@
       <c r="V9" s="8"/>
       <c r="W9" s="20"/>
       <c r="X9" s="26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Y9" s="22"/>
       <c r="Z9" s="7"/>
       <c r="AA9" s="27"/>
-      <c r="AB9" s="28"/>
+      <c r="AB9" s="21"/>
       <c r="AC9" s="20"/>
       <c r="AD9" s="27"/>
       <c r="AE9" s="27"/>
@@ -1520,7 +1573,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="7"/>
@@ -1532,7 +1585,7 @@
       <c r="N10" s="7"/>
       <c r="O10" s="17"/>
       <c r="P10" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Q10" s="8"/>
       <c r="R10" s="18"/>
@@ -1541,18 +1594,18 @@
       <c r="U10" s="19"/>
       <c r="V10" s="8"/>
       <c r="W10" s="20"/>
-      <c r="X10" s="29" t="s">
-        <v>41</v>
+      <c r="X10" s="28" t="s">
+        <v>42</v>
       </c>
       <c r="Y10" s="22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Z10" s="7"/>
       <c r="AA10" s="8"/>
-      <c r="AB10" s="28"/>
+      <c r="AB10" s="21"/>
       <c r="AC10" s="20"/>
       <c r="AD10" s="22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AE10" s="22"/>
       <c r="AF10" s="8"/>
@@ -1560,63 +1613,65 @@
     <row r="11" customFormat="false" ht="23.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="2"/>
       <c r="B11" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="31" t="s">
         <v>45</v>
       </c>
+      <c r="C11" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>47</v>
+      </c>
       <c r="E11" s="12"/>
-      <c r="F11" s="32" t="s">
-        <v>28</v>
+      <c r="F11" s="31" t="s">
+        <v>29</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="7"/>
       <c r="I11" s="23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K11" s="8"/>
       <c r="L11" s="16" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="M11" s="23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N11" s="7"/>
       <c r="O11" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P11" s="24" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q11" s="8"/>
       <c r="R11" s="18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="S11" s="8"/>
       <c r="T11" s="7"/>
       <c r="U11" s="19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="V11" s="8"/>
       <c r="W11" s="20"/>
       <c r="X11" s="26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Y11" s="22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Z11" s="7"/>
       <c r="AA11" s="8"/>
       <c r="AB11" s="21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AC11" s="20"/>
       <c r="AD11" s="27" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AE11" s="27"/>
       <c r="AF11" s="8"/>
@@ -1625,12 +1680,12 @@
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="34"/>
-      <c r="F12" s="29" t="s">
-        <v>49</v>
+      <c r="D12" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="33"/>
+      <c r="F12" s="28" t="s">
+        <v>51</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="7"/>
@@ -1642,7 +1697,7 @@
       <c r="N12" s="7"/>
       <c r="O12" s="17"/>
       <c r="P12" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q12" s="8"/>
       <c r="R12" s="18"/>
@@ -1652,7 +1707,7 @@
       <c r="V12" s="8"/>
       <c r="W12" s="20"/>
       <c r="X12" s="26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Y12" s="22"/>
       <c r="Z12" s="7"/>
@@ -1667,11 +1722,11 @@
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" s="34"/>
-      <c r="F13" s="29"/>
+      <c r="D13" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="33"/>
+      <c r="F13" s="28"/>
       <c r="G13" s="8"/>
       <c r="H13" s="7"/>
       <c r="I13" s="23"/>
@@ -1682,7 +1737,7 @@
       <c r="N13" s="7"/>
       <c r="O13" s="17"/>
       <c r="P13" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Q13" s="8"/>
       <c r="R13" s="18"/>
@@ -1691,18 +1746,18 @@
       <c r="U13" s="19"/>
       <c r="V13" s="8"/>
       <c r="W13" s="20"/>
-      <c r="X13" s="29" t="s">
-        <v>41</v>
+      <c r="X13" s="28" t="s">
+        <v>42</v>
       </c>
       <c r="Y13" s="22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Z13" s="7"/>
       <c r="AA13" s="8"/>
       <c r="AB13" s="21"/>
       <c r="AC13" s="20"/>
       <c r="AD13" s="22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AE13" s="22"/>
       <c r="AF13" s="8"/>
@@ -1711,10 +1766,10 @@
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="33"/>
       <c r="F14" s="27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G14" s="8"/>
       <c r="H14" s="7"/>
@@ -1733,7 +1788,7 @@
       <c r="U14" s="19"/>
       <c r="V14" s="8"/>
       <c r="W14" s="20"/>
-      <c r="X14" s="29"/>
+      <c r="X14" s="28"/>
       <c r="Y14" s="22"/>
       <c r="Z14" s="7"/>
       <c r="AA14" s="8"/>
@@ -1746,63 +1801,65 @@
     <row r="15" customFormat="false" ht="23.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="2"/>
       <c r="B15" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="31" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>54</v>
       </c>
       <c r="E15" s="12"/>
-      <c r="F15" s="32" t="s">
-        <v>28</v>
+      <c r="F15" s="31" t="s">
+        <v>29</v>
       </c>
       <c r="G15" s="8"/>
       <c r="H15" s="7"/>
       <c r="I15" s="23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J15" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K15" s="8"/>
       <c r="L15" s="16" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="M15" s="23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N15" s="7"/>
       <c r="O15" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P15" s="24" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q15" s="8"/>
       <c r="R15" s="18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="S15" s="8"/>
       <c r="T15" s="7"/>
       <c r="U15" s="19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="V15" s="8"/>
       <c r="W15" s="20"/>
       <c r="X15" s="26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Y15" s="22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Z15" s="7"/>
       <c r="AA15" s="8"/>
       <c r="AB15" s="21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AC15" s="20"/>
       <c r="AD15" s="27" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AE15" s="27"/>
       <c r="AF15" s="8"/>
@@ -1811,12 +1868,12 @@
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" s="34"/>
-      <c r="F16" s="29" t="s">
-        <v>53</v>
+      <c r="D16" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="33"/>
+      <c r="F16" s="28" t="s">
+        <v>55</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="7"/>
@@ -1828,7 +1885,7 @@
       <c r="N16" s="7"/>
       <c r="O16" s="17"/>
       <c r="P16" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q16" s="8"/>
       <c r="R16" s="18"/>
@@ -1838,7 +1895,7 @@
       <c r="V16" s="8"/>
       <c r="W16" s="20"/>
       <c r="X16" s="26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Y16" s="22"/>
       <c r="Z16" s="7"/>
@@ -1853,11 +1910,11 @@
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" s="34"/>
-      <c r="F17" s="29"/>
+      <c r="D17" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="33"/>
+      <c r="F17" s="28"/>
       <c r="G17" s="8"/>
       <c r="H17" s="7"/>
       <c r="I17" s="23"/>
@@ -1868,7 +1925,7 @@
       <c r="N17" s="7"/>
       <c r="O17" s="17"/>
       <c r="P17" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Q17" s="8"/>
       <c r="R17" s="18"/>
@@ -1877,18 +1934,18 @@
       <c r="U17" s="19"/>
       <c r="V17" s="8"/>
       <c r="W17" s="20"/>
-      <c r="X17" s="29" t="s">
-        <v>54</v>
+      <c r="X17" s="28" t="s">
+        <v>56</v>
       </c>
       <c r="Y17" s="22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Z17" s="7"/>
       <c r="AA17" s="8"/>
       <c r="AB17" s="21"/>
       <c r="AC17" s="20"/>
       <c r="AD17" s="22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AE17" s="22"/>
       <c r="AF17" s="8"/>
@@ -1897,10 +1954,10 @@
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="33"/>
       <c r="F18" s="27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="7"/>
@@ -1919,7 +1976,7 @@
       <c r="U18" s="19"/>
       <c r="V18" s="8"/>
       <c r="W18" s="20"/>
-      <c r="X18" s="29"/>
+      <c r="X18" s="28"/>
       <c r="Y18" s="22"/>
       <c r="Z18" s="7"/>
       <c r="AA18" s="8"/>
@@ -1932,61 +1989,63 @@
     <row r="19" customFormat="false" ht="23.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="2"/>
       <c r="B19" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="31" t="s">
-        <v>45</v>
+        <v>57</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>47</v>
       </c>
       <c r="E19" s="12"/>
-      <c r="F19" s="32" t="s">
-        <v>28</v>
+      <c r="F19" s="31" t="s">
+        <v>29</v>
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="7"/>
       <c r="I19" s="23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J19" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
       <c r="M19" s="23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N19" s="7"/>
       <c r="O19" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P19" s="24" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q19" s="8"/>
       <c r="R19" s="18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="S19" s="8"/>
       <c r="T19" s="7"/>
       <c r="U19" s="19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="V19" s="8"/>
-      <c r="W19" s="34"/>
+      <c r="W19" s="33"/>
       <c r="X19" s="26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Y19" s="22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Z19" s="7"/>
       <c r="AA19" s="8"/>
       <c r="AB19" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC19" s="34"/>
+        <v>27</v>
+      </c>
+      <c r="AC19" s="33"/>
       <c r="AD19" s="27" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AE19" s="27"/>
       <c r="AF19" s="8"/>
@@ -1995,12 +2054,12 @@
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" s="34"/>
-      <c r="F20" s="29" t="s">
-        <v>49</v>
+      <c r="D20" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="33"/>
+      <c r="F20" s="28" t="s">
+        <v>51</v>
       </c>
       <c r="G20" s="8"/>
       <c r="H20" s="7"/>
@@ -2012,7 +2071,7 @@
       <c r="N20" s="7"/>
       <c r="O20" s="17"/>
       <c r="P20" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q20" s="8"/>
       <c r="R20" s="18"/>
@@ -2020,15 +2079,15 @@
       <c r="T20" s="7"/>
       <c r="U20" s="19"/>
       <c r="V20" s="8"/>
-      <c r="W20" s="34"/>
+      <c r="W20" s="33"/>
       <c r="X20" s="26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Y20" s="22"/>
       <c r="Z20" s="7"/>
       <c r="AA20" s="8"/>
       <c r="AB20" s="21"/>
-      <c r="AC20" s="34"/>
+      <c r="AC20" s="33"/>
       <c r="AD20" s="27"/>
       <c r="AE20" s="27"/>
       <c r="AF20" s="8"/>
@@ -2037,11 +2096,11 @@
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="E21" s="34"/>
-      <c r="F21" s="29"/>
+      <c r="D21" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="33"/>
+      <c r="F21" s="28"/>
       <c r="G21" s="8"/>
       <c r="H21" s="7"/>
       <c r="I21" s="23"/>
@@ -2052,7 +2111,7 @@
       <c r="N21" s="7"/>
       <c r="O21" s="17"/>
       <c r="P21" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Q21" s="8"/>
       <c r="R21" s="18"/>
@@ -2060,19 +2119,19 @@
       <c r="T21" s="7"/>
       <c r="U21" s="19"/>
       <c r="V21" s="8"/>
-      <c r="W21" s="34"/>
-      <c r="X21" s="29" t="s">
-        <v>41</v>
+      <c r="W21" s="33"/>
+      <c r="X21" s="28" t="s">
+        <v>42</v>
       </c>
       <c r="Y21" s="22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Z21" s="7"/>
       <c r="AA21" s="8"/>
       <c r="AB21" s="21"/>
-      <c r="AC21" s="34"/>
+      <c r="AC21" s="33"/>
       <c r="AD21" s="22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AE21" s="22"/>
       <c r="AF21" s="8"/>
@@ -2081,10 +2140,10 @@
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="33"/>
       <c r="F22" s="27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G22" s="8"/>
       <c r="H22" s="7"/>
@@ -2102,13 +2161,13 @@
       <c r="T22" s="7"/>
       <c r="U22" s="19"/>
       <c r="V22" s="8"/>
-      <c r="W22" s="34"/>
-      <c r="X22" s="29"/>
+      <c r="W22" s="33"/>
+      <c r="X22" s="28"/>
       <c r="Y22" s="22"/>
       <c r="Z22" s="7"/>
       <c r="AA22" s="8"/>
       <c r="AB22" s="21"/>
-      <c r="AC22" s="34"/>
+      <c r="AC22" s="33"/>
       <c r="AD22" s="22"/>
       <c r="AE22" s="22"/>
       <c r="AF22" s="8"/>
@@ -2116,61 +2175,63 @@
     <row r="23" customFormat="false" ht="22.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="2"/>
       <c r="B23" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C23" s="30"/>
-      <c r="D23" s="31" t="s">
-        <v>45</v>
+        <v>59</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>47</v>
       </c>
       <c r="E23" s="12"/>
-      <c r="F23" s="32" t="s">
-        <v>28</v>
+      <c r="F23" s="31" t="s">
+        <v>29</v>
       </c>
       <c r="G23" s="8"/>
       <c r="H23" s="7"/>
       <c r="I23" s="23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J23" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
       <c r="M23" s="23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N23" s="7"/>
       <c r="O23" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P23" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q23" s="8"/>
       <c r="R23" s="18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="S23" s="8"/>
       <c r="T23" s="7"/>
       <c r="U23" s="19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="V23" s="8"/>
       <c r="W23" s="8"/>
       <c r="X23" s="26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Y23" s="22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Z23" s="7"/>
       <c r="AA23" s="8"/>
       <c r="AB23" s="21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AC23" s="8"/>
       <c r="AD23" s="27" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AE23" s="27"/>
       <c r="AF23" s="8"/>
@@ -2179,12 +2240,12 @@
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="E24" s="34"/>
-      <c r="F24" s="29" t="s">
-        <v>49</v>
+      <c r="D24" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="33"/>
+      <c r="F24" s="28" t="s">
+        <v>51</v>
       </c>
       <c r="G24" s="8"/>
       <c r="H24" s="7"/>
@@ -2204,7 +2265,7 @@
       <c r="V24" s="8"/>
       <c r="W24" s="8"/>
       <c r="X24" s="26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Y24" s="22"/>
       <c r="Z24" s="7"/>
@@ -2219,11 +2280,11 @@
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="E25" s="34"/>
-      <c r="F25" s="29"/>
+      <c r="D25" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" s="33"/>
+      <c r="F25" s="28"/>
       <c r="G25" s="8"/>
       <c r="H25" s="7"/>
       <c r="I25" s="23"/>
@@ -2234,7 +2295,7 @@
       <c r="N25" s="7"/>
       <c r="O25" s="17"/>
       <c r="P25" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Q25" s="8"/>
       <c r="R25" s="18"/>
@@ -2243,18 +2304,18 @@
       <c r="U25" s="19"/>
       <c r="V25" s="8"/>
       <c r="W25" s="8"/>
-      <c r="X25" s="29" t="s">
-        <v>58</v>
+      <c r="X25" s="28" t="s">
+        <v>60</v>
       </c>
       <c r="Y25" s="22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Z25" s="7"/>
       <c r="AA25" s="8"/>
       <c r="AB25" s="21"/>
       <c r="AC25" s="8"/>
       <c r="AD25" s="22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AE25" s="22"/>
       <c r="AF25" s="8"/>
@@ -2263,10 +2324,10 @@
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="33"/>
       <c r="F26" s="27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G26" s="8"/>
       <c r="H26" s="7"/>
@@ -2285,7 +2346,7 @@
       <c r="U26" s="19"/>
       <c r="V26" s="8"/>
       <c r="W26" s="8"/>
-      <c r="X26" s="29"/>
+      <c r="X26" s="28"/>
       <c r="Y26" s="22"/>
       <c r="Z26" s="7"/>
       <c r="AA26" s="8"/>
@@ -2298,181 +2359,181 @@
     <row r="27" customFormat="false" ht="17.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="2"/>
       <c r="B27" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+        <v>61</v>
+      </c>
+      <c r="C27" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="35"/>
       <c r="K27" s="8"/>
-      <c r="L27" s="37" t="s">
-        <v>61</v>
-      </c>
-      <c r="M27" s="37"/>
+      <c r="L27" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="M27" s="36"/>
       <c r="N27" s="7"/>
-      <c r="O27" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="P27" s="38"/>
-      <c r="Q27" s="38"/>
-      <c r="R27" s="38"/>
-      <c r="S27" s="38"/>
-      <c r="T27" s="38"/>
-      <c r="U27" s="38"/>
-      <c r="V27" s="38"/>
-      <c r="W27" s="38"/>
-      <c r="X27" s="38"/>
-      <c r="Y27" s="38"/>
-      <c r="Z27" s="38"/>
-      <c r="AA27" s="38"/>
-      <c r="AB27" s="38"/>
-      <c r="AC27" s="38"/>
-      <c r="AD27" s="38"/>
-      <c r="AE27" s="38"/>
-      <c r="AF27" s="38"/>
+      <c r="O27" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="P27" s="37"/>
+      <c r="Q27" s="37"/>
+      <c r="R27" s="37"/>
+      <c r="S27" s="37"/>
+      <c r="T27" s="37"/>
+      <c r="U27" s="37"/>
+      <c r="V27" s="37"/>
+      <c r="W27" s="37"/>
+      <c r="X27" s="37"/>
+      <c r="Y27" s="37"/>
+      <c r="Z27" s="37"/>
+      <c r="AA27" s="37"/>
+      <c r="AB27" s="37"/>
+      <c r="AC27" s="37"/>
+      <c r="AD27" s="37"/>
+      <c r="AE27" s="37"/>
+      <c r="AF27" s="37"/>
     </row>
     <row r="28" customFormat="false" ht="17.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="35"/>
+      <c r="J28" s="35"/>
       <c r="K28" s="8"/>
-      <c r="L28" s="37"/>
-      <c r="M28" s="37"/>
+      <c r="L28" s="36"/>
+      <c r="M28" s="36"/>
       <c r="N28" s="7"/>
-      <c r="O28" s="38"/>
-      <c r="P28" s="38"/>
-      <c r="Q28" s="38"/>
-      <c r="R28" s="38"/>
-      <c r="S28" s="38"/>
-      <c r="T28" s="38"/>
-      <c r="U28" s="38"/>
-      <c r="V28" s="38"/>
-      <c r="W28" s="38"/>
-      <c r="X28" s="38"/>
-      <c r="Y28" s="38"/>
-      <c r="Z28" s="38"/>
-      <c r="AA28" s="38"/>
-      <c r="AB28" s="38"/>
-      <c r="AC28" s="38"/>
-      <c r="AD28" s="38"/>
-      <c r="AE28" s="38"/>
-      <c r="AF28" s="38"/>
+      <c r="O28" s="37"/>
+      <c r="P28" s="37"/>
+      <c r="Q28" s="37"/>
+      <c r="R28" s="37"/>
+      <c r="S28" s="37"/>
+      <c r="T28" s="37"/>
+      <c r="U28" s="37"/>
+      <c r="V28" s="37"/>
+      <c r="W28" s="37"/>
+      <c r="X28" s="37"/>
+      <c r="Y28" s="37"/>
+      <c r="Z28" s="37"/>
+      <c r="AA28" s="37"/>
+      <c r="AB28" s="37"/>
+      <c r="AC28" s="37"/>
+      <c r="AD28" s="37"/>
+      <c r="AE28" s="37"/>
+      <c r="AF28" s="37"/>
     </row>
     <row r="29" customFormat="false" ht="71.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="2"/>
       <c r="B29" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="39"/>
-      <c r="M29" s="39"/>
-      <c r="N29" s="39"/>
-      <c r="O29" s="39"/>
-      <c r="P29" s="39"/>
-      <c r="Q29" s="39"/>
-      <c r="R29" s="39"/>
-      <c r="S29" s="39"/>
-      <c r="T29" s="39"/>
-      <c r="U29" s="39"/>
-      <c r="V29" s="39"/>
-      <c r="W29" s="39"/>
-      <c r="X29" s="39"/>
-      <c r="Y29" s="39"/>
-      <c r="Z29" s="39"/>
-      <c r="AA29" s="39"/>
-      <c r="AB29" s="39"/>
-      <c r="AC29" s="39"/>
-      <c r="AD29" s="39"/>
-      <c r="AE29" s="39"/>
-      <c r="AF29" s="39"/>
+        <v>64</v>
+      </c>
+      <c r="C29" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
+      <c r="K29" s="38"/>
+      <c r="L29" s="38"/>
+      <c r="M29" s="38"/>
+      <c r="N29" s="38"/>
+      <c r="O29" s="38"/>
+      <c r="P29" s="38"/>
+      <c r="Q29" s="38"/>
+      <c r="R29" s="38"/>
+      <c r="S29" s="38"/>
+      <c r="T29" s="38"/>
+      <c r="U29" s="38"/>
+      <c r="V29" s="38"/>
+      <c r="W29" s="38"/>
+      <c r="X29" s="38"/>
+      <c r="Y29" s="38"/>
+      <c r="Z29" s="38"/>
+      <c r="AA29" s="38"/>
+      <c r="AB29" s="38"/>
+      <c r="AC29" s="38"/>
+      <c r="AD29" s="38"/>
+      <c r="AE29" s="38"/>
+      <c r="AF29" s="38"/>
     </row>
     <row r="30" customFormat="false" ht="23.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="2"/>
       <c r="B30" s="10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C30" s="8"/>
-      <c r="D30" s="29" t="s">
-        <v>45</v>
+      <c r="D30" s="28" t="s">
+        <v>47</v>
       </c>
       <c r="E30" s="8"/>
-      <c r="F30" s="32" t="s">
-        <v>28</v>
+      <c r="F30" s="31" t="s">
+        <v>29</v>
       </c>
       <c r="G30" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H30" s="7"/>
       <c r="I30" s="23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J30" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K30" s="8"/>
       <c r="L30" s="16" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="M30" s="16" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="N30" s="7"/>
       <c r="O30" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P30" s="24" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q30" s="8"/>
       <c r="R30" s="18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="S30" s="8"/>
       <c r="T30" s="7"/>
       <c r="U30" s="19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="V30" s="8"/>
       <c r="W30" s="8"/>
       <c r="X30" s="26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Y30" s="22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Z30" s="7"/>
       <c r="AA30" s="23" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AB30" s="21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AC30" s="8"/>
       <c r="AD30" s="27" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AE30" s="27"/>
       <c r="AF30" s="8"/>
@@ -2481,10 +2542,10 @@
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="29"/>
+      <c r="D31" s="28"/>
       <c r="E31" s="8"/>
-      <c r="F31" s="29" t="s">
-        <v>49</v>
+      <c r="F31" s="28" t="s">
+        <v>51</v>
       </c>
       <c r="G31" s="23"/>
       <c r="H31" s="7"/>
@@ -2496,7 +2557,7 @@
       <c r="N31" s="7"/>
       <c r="O31" s="17"/>
       <c r="P31" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q31" s="8"/>
       <c r="R31" s="18"/>
@@ -2506,7 +2567,7 @@
       <c r="V31" s="8"/>
       <c r="W31" s="8"/>
       <c r="X31" s="26" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Y31" s="22"/>
       <c r="Z31" s="7"/>
@@ -2521,9 +2582,9 @@
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="29"/>
+      <c r="D32" s="28"/>
       <c r="E32" s="8"/>
-      <c r="F32" s="29"/>
+      <c r="F32" s="28"/>
       <c r="G32" s="23"/>
       <c r="H32" s="7"/>
       <c r="I32" s="23"/>
@@ -2534,7 +2595,7 @@
       <c r="N32" s="7"/>
       <c r="O32" s="17"/>
       <c r="P32" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Q32" s="8"/>
       <c r="R32" s="18"/>
@@ -2543,18 +2604,18 @@
       <c r="U32" s="19"/>
       <c r="V32" s="8"/>
       <c r="W32" s="8"/>
-      <c r="X32" s="29" t="s">
-        <v>58</v>
+      <c r="X32" s="28" t="s">
+        <v>60</v>
       </c>
       <c r="Y32" s="22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Z32" s="7"/>
       <c r="AA32" s="23"/>
       <c r="AB32" s="21"/>
       <c r="AC32" s="8"/>
       <c r="AD32" s="22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AE32" s="22"/>
       <c r="AF32" s="8"/>
@@ -2563,10 +2624,10 @@
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="29"/>
+      <c r="D33" s="28"/>
       <c r="E33" s="8"/>
       <c r="F33" s="27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G33" s="23"/>
       <c r="H33" s="7"/>
@@ -2585,7 +2646,7 @@
       <c r="U33" s="19"/>
       <c r="V33" s="8"/>
       <c r="W33" s="8"/>
-      <c r="X33" s="29"/>
+      <c r="X33" s="28"/>
       <c r="Y33" s="22"/>
       <c r="Z33" s="7"/>
       <c r="AA33" s="23"/>
@@ -2598,61 +2659,63 @@
     <row r="34" customFormat="false" ht="22.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="2"/>
       <c r="B34" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="C34" s="30"/>
-      <c r="D34" s="31" t="s">
-        <v>52</v>
+        <v>70</v>
+      </c>
+      <c r="C34" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="30" t="s">
+        <v>54</v>
       </c>
       <c r="E34" s="12"/>
-      <c r="F34" s="32" t="s">
-        <v>28</v>
+      <c r="F34" s="31" t="s">
+        <v>29</v>
       </c>
       <c r="G34" s="8"/>
       <c r="H34" s="7"/>
       <c r="I34" s="23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J34" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K34" s="8"/>
       <c r="L34" s="16" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="M34" s="23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N34" s="7"/>
       <c r="O34" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="P34" s="3"/>
       <c r="Q34" s="8"/>
       <c r="R34" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="S34" s="3"/>
       <c r="T34" s="7"/>
       <c r="U34" s="19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="V34" s="8"/>
       <c r="W34" s="8"/>
       <c r="X34" s="26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Y34" s="22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Z34" s="7"/>
       <c r="AA34" s="8"/>
       <c r="AB34" s="21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AC34" s="8"/>
       <c r="AD34" s="27" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AE34" s="27"/>
       <c r="AF34" s="8"/>
@@ -2661,12 +2724,12 @@
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
-      <c r="D35" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="E35" s="34"/>
-      <c r="F35" s="29" t="s">
-        <v>53</v>
+      <c r="D35" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="E35" s="33"/>
+      <c r="F35" s="28" t="s">
+        <v>55</v>
       </c>
       <c r="G35" s="8"/>
       <c r="H35" s="7"/>
@@ -2686,7 +2749,7 @@
       <c r="V35" s="8"/>
       <c r="W35" s="8"/>
       <c r="X35" s="26" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Y35" s="22"/>
       <c r="Z35" s="7"/>
@@ -2701,11 +2764,11 @@
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
-      <c r="D36" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="29"/>
+      <c r="D36" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="E36" s="33"/>
+      <c r="F36" s="28"/>
       <c r="G36" s="8"/>
       <c r="H36" s="7"/>
       <c r="I36" s="23"/>
@@ -2723,18 +2786,18 @@
       <c r="U36" s="19"/>
       <c r="V36" s="8"/>
       <c r="W36" s="8"/>
-      <c r="X36" s="29" t="s">
-        <v>71</v>
+      <c r="X36" s="28" t="s">
+        <v>73</v>
       </c>
       <c r="Y36" s="22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Z36" s="7"/>
       <c r="AA36" s="8"/>
       <c r="AB36" s="21"/>
       <c r="AC36" s="8"/>
       <c r="AD36" s="22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AE36" s="22"/>
       <c r="AF36" s="8"/>
@@ -2743,10 +2806,10 @@
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="34"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="33"/>
       <c r="F37" s="27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G37" s="8"/>
       <c r="H37" s="7"/>
@@ -2765,7 +2828,7 @@
       <c r="U37" s="19"/>
       <c r="V37" s="8"/>
       <c r="W37" s="8"/>
-      <c r="X37" s="29"/>
+      <c r="X37" s="28"/>
       <c r="Y37" s="22"/>
       <c r="Z37" s="7"/>
       <c r="AA37" s="8"/>
@@ -2778,63 +2841,65 @@
     <row r="38" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="2"/>
       <c r="B38" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C38" s="30"/>
-      <c r="D38" s="31" t="s">
-        <v>45</v>
+        <v>74</v>
+      </c>
+      <c r="C38" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D38" s="30" t="s">
+        <v>47</v>
       </c>
       <c r="E38" s="12"/>
-      <c r="F38" s="32" t="s">
-        <v>28</v>
+      <c r="F38" s="31" t="s">
+        <v>29</v>
       </c>
       <c r="G38" s="8"/>
       <c r="H38" s="7"/>
       <c r="I38" s="23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J38" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K38" s="8"/>
       <c r="L38" s="16" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="M38" s="23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N38" s="7"/>
       <c r="O38" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P38" s="24" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q38" s="8"/>
       <c r="R38" s="18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="S38" s="8"/>
       <c r="T38" s="7"/>
       <c r="U38" s="19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="V38" s="8"/>
       <c r="W38" s="8"/>
       <c r="X38" s="26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Y38" s="22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Z38" s="7"/>
       <c r="AA38" s="8"/>
       <c r="AB38" s="21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AC38" s="8"/>
       <c r="AD38" s="27" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AE38" s="27"/>
       <c r="AF38" s="8"/>
@@ -2843,12 +2908,12 @@
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
-      <c r="D39" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="E39" s="34"/>
-      <c r="F39" s="29" t="s">
-        <v>49</v>
+      <c r="D39" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="E39" s="33"/>
+      <c r="F39" s="28" t="s">
+        <v>51</v>
       </c>
       <c r="G39" s="8"/>
       <c r="H39" s="7"/>
@@ -2860,7 +2925,7 @@
       <c r="N39" s="7"/>
       <c r="O39" s="17"/>
       <c r="P39" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q39" s="8"/>
       <c r="R39" s="18"/>
@@ -2870,7 +2935,7 @@
       <c r="V39" s="8"/>
       <c r="W39" s="8"/>
       <c r="X39" s="26" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Y39" s="22"/>
       <c r="Z39" s="7"/>
@@ -2885,11 +2950,11 @@
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
-      <c r="D40" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="E40" s="34"/>
-      <c r="F40" s="29"/>
+      <c r="D40" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="E40" s="33"/>
+      <c r="F40" s="28"/>
       <c r="G40" s="8"/>
       <c r="H40" s="7"/>
       <c r="I40" s="23"/>
@@ -2900,7 +2965,7 @@
       <c r="N40" s="7"/>
       <c r="O40" s="17"/>
       <c r="P40" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Q40" s="8"/>
       <c r="R40" s="18"/>
@@ -2909,18 +2974,18 @@
       <c r="U40" s="19"/>
       <c r="V40" s="8"/>
       <c r="W40" s="8"/>
-      <c r="X40" s="29" t="s">
-        <v>58</v>
+      <c r="X40" s="28" t="s">
+        <v>60</v>
       </c>
       <c r="Y40" s="22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Z40" s="7"/>
       <c r="AA40" s="8"/>
       <c r="AB40" s="21"/>
       <c r="AC40" s="8"/>
       <c r="AD40" s="22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AE40" s="22"/>
       <c r="AF40" s="8"/>
@@ -2929,10 +2994,10 @@
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
-      <c r="D41" s="35"/>
-      <c r="E41" s="34"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="33"/>
       <c r="F41" s="27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G41" s="8"/>
       <c r="H41" s="7"/>
@@ -2951,7 +3016,7 @@
       <c r="U41" s="19"/>
       <c r="V41" s="8"/>
       <c r="W41" s="8"/>
-      <c r="X41" s="29"/>
+      <c r="X41" s="28"/>
       <c r="Y41" s="22"/>
       <c r="Z41" s="7"/>
       <c r="AA41" s="8"/>
@@ -2964,63 +3029,65 @@
     <row r="42" customFormat="false" ht="23.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="2"/>
       <c r="B42" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C42" s="30"/>
-      <c r="D42" s="31" t="s">
-        <v>45</v>
+        <v>75</v>
+      </c>
+      <c r="C42" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D42" s="30" t="s">
+        <v>47</v>
       </c>
       <c r="E42" s="12"/>
-      <c r="F42" s="32" t="s">
-        <v>28</v>
+      <c r="F42" s="31" t="s">
+        <v>29</v>
       </c>
       <c r="G42" s="8"/>
       <c r="H42" s="7"/>
       <c r="I42" s="23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J42" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K42" s="8"/>
       <c r="L42" s="16" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="M42" s="23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N42" s="7"/>
       <c r="O42" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P42" s="24" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q42" s="8"/>
       <c r="R42" s="18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="S42" s="8"/>
       <c r="T42" s="7"/>
       <c r="U42" s="19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="V42" s="8"/>
       <c r="W42" s="8"/>
       <c r="X42" s="26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Y42" s="22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Z42" s="7"/>
       <c r="AA42" s="8"/>
       <c r="AB42" s="21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AC42" s="8"/>
       <c r="AD42" s="27" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AE42" s="27"/>
       <c r="AF42" s="8"/>
@@ -3029,12 +3096,12 @@
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
-      <c r="D43" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="E43" s="34"/>
-      <c r="F43" s="29" t="s">
-        <v>49</v>
+      <c r="D43" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="E43" s="33"/>
+      <c r="F43" s="28" t="s">
+        <v>51</v>
       </c>
       <c r="G43" s="8"/>
       <c r="H43" s="7"/>
@@ -3046,7 +3113,7 @@
       <c r="N43" s="7"/>
       <c r="O43" s="17"/>
       <c r="P43" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q43" s="8"/>
       <c r="R43" s="18"/>
@@ -3056,7 +3123,7 @@
       <c r="V43" s="8"/>
       <c r="W43" s="8"/>
       <c r="X43" s="26" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Y43" s="22"/>
       <c r="Z43" s="7"/>
@@ -3071,11 +3138,11 @@
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
-      <c r="D44" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="E44" s="34"/>
-      <c r="F44" s="29"/>
+      <c r="D44" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="E44" s="33"/>
+      <c r="F44" s="28"/>
       <c r="G44" s="8"/>
       <c r="H44" s="7"/>
       <c r="I44" s="23"/>
@@ -3086,7 +3153,7 @@
       <c r="N44" s="7"/>
       <c r="O44" s="17"/>
       <c r="P44" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Q44" s="8"/>
       <c r="R44" s="18"/>
@@ -3095,18 +3162,18 @@
       <c r="U44" s="19"/>
       <c r="V44" s="8"/>
       <c r="W44" s="8"/>
-      <c r="X44" s="29" t="s">
-        <v>58</v>
+      <c r="X44" s="28" t="s">
+        <v>60</v>
       </c>
       <c r="Y44" s="22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Z44" s="7"/>
       <c r="AA44" s="8"/>
       <c r="AB44" s="21"/>
       <c r="AC44" s="8"/>
       <c r="AD44" s="22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AE44" s="22"/>
       <c r="AF44" s="8"/>
@@ -3115,10 +3182,10 @@
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="35"/>
-      <c r="E45" s="34"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="33"/>
       <c r="F45" s="27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G45" s="8"/>
       <c r="H45" s="7"/>
@@ -3137,7 +3204,7 @@
       <c r="U45" s="19"/>
       <c r="V45" s="8"/>
       <c r="W45" s="8"/>
-      <c r="X45" s="29"/>
+      <c r="X45" s="28"/>
       <c r="Y45" s="22"/>
       <c r="Z45" s="7"/>
       <c r="AA45" s="8"/>
@@ -3150,61 +3217,63 @@
     <row r="46" customFormat="false" ht="23.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="2"/>
       <c r="B46" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C46" s="30"/>
-      <c r="D46" s="31" t="s">
-        <v>45</v>
+        <v>76</v>
+      </c>
+      <c r="C46" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D46" s="30" t="s">
+        <v>47</v>
       </c>
       <c r="E46" s="12"/>
-      <c r="F46" s="32" t="s">
-        <v>28</v>
+      <c r="F46" s="31" t="s">
+        <v>29</v>
       </c>
       <c r="G46" s="8"/>
       <c r="H46" s="7"/>
       <c r="I46" s="23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J46" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K46" s="8"/>
       <c r="L46" s="8"/>
       <c r="M46" s="23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N46" s="7"/>
       <c r="O46" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P46" s="24" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q46" s="8"/>
       <c r="R46" s="18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="S46" s="8"/>
       <c r="T46" s="7"/>
       <c r="U46" s="19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="V46" s="8"/>
       <c r="W46" s="8"/>
       <c r="X46" s="26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Y46" s="22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Z46" s="7"/>
       <c r="AA46" s="8"/>
       <c r="AB46" s="21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AC46" s="8"/>
       <c r="AD46" s="27" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AE46" s="27"/>
       <c r="AF46" s="8"/>
@@ -3213,12 +3282,12 @@
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
-      <c r="D47" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="E47" s="34"/>
-      <c r="F47" s="29" t="s">
-        <v>49</v>
+      <c r="D47" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="E47" s="33"/>
+      <c r="F47" s="28" t="s">
+        <v>51</v>
       </c>
       <c r="G47" s="8"/>
       <c r="H47" s="7"/>
@@ -3230,7 +3299,7 @@
       <c r="N47" s="7"/>
       <c r="O47" s="17"/>
       <c r="P47" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q47" s="8"/>
       <c r="R47" s="18"/>
@@ -3240,7 +3309,7 @@
       <c r="V47" s="8"/>
       <c r="W47" s="8"/>
       <c r="X47" s="26" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Y47" s="22"/>
       <c r="Z47" s="7"/>
@@ -3255,11 +3324,11 @@
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
-      <c r="D48" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="E48" s="34"/>
-      <c r="F48" s="29"/>
+      <c r="D48" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="E48" s="33"/>
+      <c r="F48" s="28"/>
       <c r="G48" s="8"/>
       <c r="H48" s="7"/>
       <c r="I48" s="23"/>
@@ -3270,7 +3339,7 @@
       <c r="N48" s="7"/>
       <c r="O48" s="17"/>
       <c r="P48" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Q48" s="8"/>
       <c r="R48" s="18"/>
@@ -3279,18 +3348,18 @@
       <c r="U48" s="19"/>
       <c r="V48" s="8"/>
       <c r="W48" s="8"/>
-      <c r="X48" s="29" t="s">
-        <v>58</v>
+      <c r="X48" s="28" t="s">
+        <v>60</v>
       </c>
       <c r="Y48" s="22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Z48" s="7"/>
       <c r="AA48" s="8"/>
       <c r="AB48" s="21"/>
       <c r="AC48" s="8"/>
       <c r="AD48" s="22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AE48" s="22"/>
       <c r="AF48" s="8"/>
@@ -3299,10 +3368,10 @@
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
-      <c r="D49" s="35"/>
-      <c r="E49" s="34"/>
+      <c r="D49" s="34"/>
+      <c r="E49" s="33"/>
       <c r="F49" s="27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G49" s="8"/>
       <c r="H49" s="7"/>
@@ -3321,7 +3390,7 @@
       <c r="U49" s="19"/>
       <c r="V49" s="8"/>
       <c r="W49" s="8"/>
-      <c r="X49" s="29"/>
+      <c r="X49" s="28"/>
       <c r="Y49" s="22"/>
       <c r="Z49" s="7"/>
       <c r="AA49" s="8"/>
@@ -3334,61 +3403,63 @@
     <row r="50" customFormat="false" ht="23.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="2"/>
       <c r="B50" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C50" s="30"/>
-      <c r="D50" s="31" t="s">
-        <v>52</v>
+        <v>77</v>
+      </c>
+      <c r="C50" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D50" s="30" t="s">
+        <v>54</v>
       </c>
       <c r="E50" s="12"/>
-      <c r="F50" s="32" t="s">
-        <v>28</v>
+      <c r="F50" s="31" t="s">
+        <v>29</v>
       </c>
       <c r="G50" s="8"/>
       <c r="H50" s="7"/>
       <c r="I50" s="23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J50" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K50" s="8"/>
       <c r="L50" s="8"/>
       <c r="M50" s="23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N50" s="7"/>
       <c r="O50" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P50" s="24" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q50" s="8"/>
       <c r="R50" s="18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="S50" s="8"/>
       <c r="T50" s="7"/>
       <c r="U50" s="19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="V50" s="8"/>
       <c r="W50" s="8"/>
       <c r="X50" s="26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Y50" s="22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Z50" s="7"/>
       <c r="AA50" s="8"/>
       <c r="AB50" s="21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AC50" s="8"/>
       <c r="AD50" s="27" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AE50" s="27"/>
       <c r="AF50" s="8"/>
@@ -3397,12 +3468,12 @@
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
-      <c r="D51" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="E51" s="34"/>
-      <c r="F51" s="29" t="s">
-        <v>53</v>
+      <c r="D51" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="E51" s="33"/>
+      <c r="F51" s="28" t="s">
+        <v>55</v>
       </c>
       <c r="G51" s="8"/>
       <c r="H51" s="7"/>
@@ -3414,7 +3485,7 @@
       <c r="N51" s="7"/>
       <c r="O51" s="17"/>
       <c r="P51" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="Q51" s="8"/>
       <c r="R51" s="18"/>
@@ -3424,7 +3495,7 @@
       <c r="V51" s="8"/>
       <c r="W51" s="8"/>
       <c r="X51" s="26" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Y51" s="22"/>
       <c r="Z51" s="7"/>
@@ -3439,11 +3510,11 @@
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
-      <c r="D52" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="E52" s="34"/>
-      <c r="F52" s="29"/>
+      <c r="D52" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="E52" s="33"/>
+      <c r="F52" s="28"/>
       <c r="G52" s="8"/>
       <c r="H52" s="7"/>
       <c r="I52" s="23"/>
@@ -3454,7 +3525,7 @@
       <c r="N52" s="7"/>
       <c r="O52" s="17"/>
       <c r="P52" s="26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Q52" s="8"/>
       <c r="R52" s="18"/>
@@ -3463,18 +3534,18 @@
       <c r="U52" s="19"/>
       <c r="V52" s="8"/>
       <c r="W52" s="8"/>
-      <c r="X52" s="29" t="s">
-        <v>71</v>
+      <c r="X52" s="28" t="s">
+        <v>73</v>
       </c>
       <c r="Y52" s="22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Z52" s="7"/>
       <c r="AA52" s="8"/>
       <c r="AB52" s="21"/>
       <c r="AC52" s="8"/>
       <c r="AD52" s="22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AE52" s="22"/>
       <c r="AF52" s="8"/>
@@ -3483,10 +3554,10 @@
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
-      <c r="D53" s="35"/>
-      <c r="E53" s="34"/>
+      <c r="D53" s="34"/>
+      <c r="E53" s="33"/>
       <c r="F53" s="27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G53" s="8"/>
       <c r="H53" s="7"/>
@@ -3505,7 +3576,7 @@
       <c r="U53" s="19"/>
       <c r="V53" s="8"/>
       <c r="W53" s="8"/>
-      <c r="X53" s="29"/>
+      <c r="X53" s="28"/>
       <c r="Y53" s="22"/>
       <c r="Z53" s="7"/>
       <c r="AA53" s="8"/>
@@ -3518,192 +3589,192 @@
     <row r="54" customFormat="false" ht="35.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="2"/>
       <c r="B54" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C54" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="D54" s="38"/>
-      <c r="E54" s="38"/>
-      <c r="F54" s="38"/>
-      <c r="G54" s="38"/>
-      <c r="H54" s="38"/>
-      <c r="I54" s="38"/>
-      <c r="J54" s="38"/>
+        <v>78</v>
+      </c>
+      <c r="C54" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="D54" s="37"/>
+      <c r="E54" s="37"/>
+      <c r="F54" s="37"/>
+      <c r="G54" s="37"/>
+      <c r="H54" s="37"/>
+      <c r="I54" s="37"/>
+      <c r="J54" s="37"/>
       <c r="K54" s="8"/>
-      <c r="L54" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="M54" s="37"/>
+      <c r="L54" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="M54" s="36"/>
       <c r="N54" s="7"/>
-      <c r="O54" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="P54" s="38"/>
-      <c r="Q54" s="38"/>
-      <c r="R54" s="38"/>
-      <c r="S54" s="38"/>
-      <c r="T54" s="38"/>
-      <c r="U54" s="38"/>
-      <c r="V54" s="38"/>
-      <c r="W54" s="38"/>
-      <c r="X54" s="38"/>
-      <c r="Y54" s="38"/>
-      <c r="Z54" s="38"/>
-      <c r="AA54" s="38"/>
-      <c r="AB54" s="38"/>
-      <c r="AC54" s="38"/>
-      <c r="AD54" s="38"/>
-      <c r="AE54" s="38"/>
-      <c r="AF54" s="38"/>
+      <c r="O54" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="P54" s="37"/>
+      <c r="Q54" s="37"/>
+      <c r="R54" s="37"/>
+      <c r="S54" s="37"/>
+      <c r="T54" s="37"/>
+      <c r="U54" s="37"/>
+      <c r="V54" s="37"/>
+      <c r="W54" s="37"/>
+      <c r="X54" s="37"/>
+      <c r="Y54" s="37"/>
+      <c r="Z54" s="37"/>
+      <c r="AA54" s="37"/>
+      <c r="AB54" s="37"/>
+      <c r="AC54" s="37"/>
+      <c r="AD54" s="37"/>
+      <c r="AE54" s="37"/>
+      <c r="AF54" s="37"/>
     </row>
     <row r="55" customFormat="false" ht="35.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="2"/>
       <c r="B55" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C55" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="D55" s="39"/>
-      <c r="E55" s="39"/>
-      <c r="F55" s="39"/>
-      <c r="G55" s="39"/>
-      <c r="H55" s="39"/>
-      <c r="I55" s="39"/>
-      <c r="J55" s="39"/>
-      <c r="K55" s="39"/>
-      <c r="L55" s="39"/>
-      <c r="M55" s="39"/>
-      <c r="N55" s="39"/>
-      <c r="O55" s="39"/>
-      <c r="P55" s="39"/>
-      <c r="Q55" s="39"/>
-      <c r="R55" s="39"/>
-      <c r="S55" s="39"/>
-      <c r="T55" s="39"/>
-      <c r="U55" s="39"/>
-      <c r="V55" s="39"/>
-      <c r="W55" s="39"/>
-      <c r="X55" s="39"/>
-      <c r="Y55" s="39"/>
-      <c r="Z55" s="39"/>
-      <c r="AA55" s="39"/>
-      <c r="AB55" s="39"/>
-      <c r="AC55" s="39"/>
-      <c r="AD55" s="39"/>
-      <c r="AE55" s="39"/>
-      <c r="AF55" s="39"/>
+        <v>81</v>
+      </c>
+      <c r="C55" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="D55" s="38"/>
+      <c r="E55" s="38"/>
+      <c r="F55" s="38"/>
+      <c r="G55" s="38"/>
+      <c r="H55" s="38"/>
+      <c r="I55" s="38"/>
+      <c r="J55" s="38"/>
+      <c r="K55" s="38"/>
+      <c r="L55" s="38"/>
+      <c r="M55" s="38"/>
+      <c r="N55" s="38"/>
+      <c r="O55" s="38"/>
+      <c r="P55" s="38"/>
+      <c r="Q55" s="38"/>
+      <c r="R55" s="38"/>
+      <c r="S55" s="38"/>
+      <c r="T55" s="38"/>
+      <c r="U55" s="38"/>
+      <c r="V55" s="38"/>
+      <c r="W55" s="38"/>
+      <c r="X55" s="38"/>
+      <c r="Y55" s="38"/>
+      <c r="Z55" s="38"/>
+      <c r="AA55" s="38"/>
+      <c r="AB55" s="38"/>
+      <c r="AC55" s="38"/>
+      <c r="AD55" s="38"/>
+      <c r="AE55" s="38"/>
+      <c r="AF55" s="38"/>
     </row>
     <row r="56" customFormat="false" ht="35.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="2"/>
       <c r="B56" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C56" s="39"/>
-      <c r="D56" s="39"/>
-      <c r="E56" s="39"/>
-      <c r="F56" s="39"/>
-      <c r="G56" s="39"/>
-      <c r="H56" s="39"/>
-      <c r="I56" s="39"/>
-      <c r="J56" s="39"/>
-      <c r="K56" s="39"/>
-      <c r="L56" s="39"/>
-      <c r="M56" s="39"/>
-      <c r="N56" s="39"/>
-      <c r="O56" s="39"/>
-      <c r="P56" s="39"/>
-      <c r="Q56" s="39"/>
-      <c r="R56" s="39"/>
-      <c r="S56" s="39"/>
-      <c r="T56" s="39"/>
-      <c r="U56" s="39"/>
-      <c r="V56" s="39"/>
-      <c r="W56" s="39"/>
-      <c r="X56" s="39"/>
-      <c r="Y56" s="39"/>
-      <c r="Z56" s="39"/>
-      <c r="AA56" s="39"/>
-      <c r="AB56" s="39"/>
-      <c r="AC56" s="39"/>
-      <c r="AD56" s="39"/>
-      <c r="AE56" s="39"/>
-      <c r="AF56" s="39"/>
+        <v>83</v>
+      </c>
+      <c r="C56" s="38"/>
+      <c r="D56" s="38"/>
+      <c r="E56" s="38"/>
+      <c r="F56" s="38"/>
+      <c r="G56" s="38"/>
+      <c r="H56" s="38"/>
+      <c r="I56" s="38"/>
+      <c r="J56" s="38"/>
+      <c r="K56" s="38"/>
+      <c r="L56" s="38"/>
+      <c r="M56" s="38"/>
+      <c r="N56" s="38"/>
+      <c r="O56" s="38"/>
+      <c r="P56" s="38"/>
+      <c r="Q56" s="38"/>
+      <c r="R56" s="38"/>
+      <c r="S56" s="38"/>
+      <c r="T56" s="38"/>
+      <c r="U56" s="38"/>
+      <c r="V56" s="38"/>
+      <c r="W56" s="38"/>
+      <c r="X56" s="38"/>
+      <c r="Y56" s="38"/>
+      <c r="Z56" s="38"/>
+      <c r="AA56" s="38"/>
+      <c r="AB56" s="38"/>
+      <c r="AC56" s="38"/>
+      <c r="AD56" s="38"/>
+      <c r="AE56" s="38"/>
+      <c r="AF56" s="38"/>
     </row>
     <row r="57" customFormat="false" ht="19.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="40" t="s">
-        <v>82</v>
-      </c>
-      <c r="B57" s="40"/>
-      <c r="C57" s="40"/>
-      <c r="D57" s="40"/>
-      <c r="E57" s="40"/>
-      <c r="F57" s="40"/>
-      <c r="G57" s="40"/>
-      <c r="H57" s="40"/>
-      <c r="I57" s="40"/>
-      <c r="J57" s="40"/>
-      <c r="K57" s="40"/>
-      <c r="L57" s="40"/>
-      <c r="M57" s="40"/>
-      <c r="N57" s="40"/>
-      <c r="O57" s="40"/>
-      <c r="P57" s="40"/>
-      <c r="Q57" s="40"/>
-      <c r="R57" s="40"/>
-      <c r="S57" s="40"/>
-      <c r="T57" s="40"/>
-      <c r="U57" s="40"/>
-      <c r="V57" s="40"/>
-      <c r="W57" s="40"/>
-      <c r="X57" s="40"/>
-      <c r="Y57" s="40"/>
-      <c r="Z57" s="40"/>
-      <c r="AA57" s="40"/>
-      <c r="AB57" s="40"/>
-      <c r="AC57" s="40"/>
-      <c r="AD57" s="40"/>
-      <c r="AE57" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="AF57" s="41"/>
-      <c r="AG57" s="41"/>
+      <c r="A57" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="B57" s="39"/>
+      <c r="C57" s="39"/>
+      <c r="D57" s="39"/>
+      <c r="E57" s="39"/>
+      <c r="F57" s="39"/>
+      <c r="G57" s="39"/>
+      <c r="H57" s="39"/>
+      <c r="I57" s="39"/>
+      <c r="J57" s="39"/>
+      <c r="K57" s="39"/>
+      <c r="L57" s="39"/>
+      <c r="M57" s="39"/>
+      <c r="N57" s="39"/>
+      <c r="O57" s="39"/>
+      <c r="P57" s="39"/>
+      <c r="Q57" s="39"/>
+      <c r="R57" s="39"/>
+      <c r="S57" s="39"/>
+      <c r="T57" s="39"/>
+      <c r="U57" s="39"/>
+      <c r="V57" s="39"/>
+      <c r="W57" s="39"/>
+      <c r="X57" s="39"/>
+      <c r="Y57" s="39"/>
+      <c r="Z57" s="39"/>
+      <c r="AA57" s="39"/>
+      <c r="AB57" s="39"/>
+      <c r="AC57" s="39"/>
+      <c r="AD57" s="39"/>
+      <c r="AE57" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="AF57" s="40"/>
+      <c r="AG57" s="40"/>
     </row>
     <row r="58" customFormat="false" ht="17.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="40"/>
-      <c r="B58" s="40"/>
-      <c r="C58" s="40"/>
-      <c r="D58" s="40"/>
-      <c r="E58" s="40"/>
-      <c r="F58" s="40"/>
-      <c r="G58" s="40"/>
-      <c r="H58" s="40"/>
-      <c r="I58" s="40"/>
-      <c r="J58" s="40"/>
-      <c r="K58" s="40"/>
-      <c r="L58" s="40"/>
-      <c r="M58" s="40"/>
-      <c r="N58" s="40"/>
-      <c r="O58" s="40"/>
-      <c r="P58" s="40"/>
-      <c r="Q58" s="40"/>
-      <c r="R58" s="40"/>
-      <c r="S58" s="40"/>
-      <c r="T58" s="40"/>
-      <c r="U58" s="40"/>
-      <c r="V58" s="40"/>
-      <c r="W58" s="40"/>
-      <c r="X58" s="40"/>
-      <c r="Y58" s="40"/>
-      <c r="Z58" s="40"/>
-      <c r="AA58" s="40"/>
-      <c r="AB58" s="40"/>
-      <c r="AC58" s="40"/>
-      <c r="AD58" s="40"/>
-      <c r="AE58" s="42"/>
-      <c r="AF58" s="42"/>
-      <c r="AG58" s="42"/>
+      <c r="A58" s="39"/>
+      <c r="B58" s="39"/>
+      <c r="C58" s="39"/>
+      <c r="D58" s="39"/>
+      <c r="E58" s="39"/>
+      <c r="F58" s="39"/>
+      <c r="G58" s="39"/>
+      <c r="H58" s="39"/>
+      <c r="I58" s="39"/>
+      <c r="J58" s="39"/>
+      <c r="K58" s="39"/>
+      <c r="L58" s="39"/>
+      <c r="M58" s="39"/>
+      <c r="N58" s="39"/>
+      <c r="O58" s="39"/>
+      <c r="P58" s="39"/>
+      <c r="Q58" s="39"/>
+      <c r="R58" s="39"/>
+      <c r="S58" s="39"/>
+      <c r="T58" s="39"/>
+      <c r="U58" s="39"/>
+      <c r="V58" s="39"/>
+      <c r="W58" s="39"/>
+      <c r="X58" s="39"/>
+      <c r="Y58" s="39"/>
+      <c r="Z58" s="39"/>
+      <c r="AA58" s="39"/>
+      <c r="AB58" s="39"/>
+      <c r="AC58" s="39"/>
+      <c r="AD58" s="39"/>
+      <c r="AE58" s="41"/>
+      <c r="AF58" s="41"/>
+      <c r="AG58" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="388">

</xml_diff>

<commit_message>
update timetables and enhance error handling
</commit_message>
<xml_diff>
--- a/assets/paris-saclay-l3-info.xlsx
+++ b/assets/paris-saclay-l3-info.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="87">
   <si>
     <r>
       <rPr>
@@ -28,7 +28,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2020/2021                                                                                                                                                                                                                                                                                                                                                                                                                                                                         </t>
     </r>
@@ -38,9 +37,8 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">11/09/2020</t>
+      <t xml:space="preserve">15/09/2020</t>
     </r>
   </si>
   <si>
@@ -105,7 +103,6 @@
         <color rgb="FFFFFFFF"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">13h30  </t>
     </r>
@@ -116,7 +113,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Réunion de rentrée
 G Amphi</t>
@@ -133,7 +129,6 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Hybride </t>
     </r>
@@ -144,7 +139,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Syst. Cours G Amphi</t>
     </r>
@@ -157,7 +151,6 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Présentiel et Hybride  </t>
     </r>
@@ -168,7 +161,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Réseau Avan. Cours G Amphi</t>
     </r>
@@ -181,7 +173,6 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Présentiel et Hybride </t>
     </r>
@@ -192,7 +183,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Réseau Avan.
 Cours G Amphi</t>
@@ -206,7 +196,6 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Présentiel et Hybride </t>
     </r>
@@ -217,7 +206,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Log. Cours
 P et  G Amphi</t>
@@ -231,7 +219,6 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Distanciel </t>
     </r>
@@ -242,7 +229,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">PFA Cours G Amphi</t>
     </r>
@@ -255,7 +241,6 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Hybride </t>
     </r>
@@ -266,7 +251,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">GLA Cours G Amphi</t>
     </r>
@@ -279,7 +263,6 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Hybride </t>
     </r>
@@ -290,7 +273,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Algo Cours G Amphi</t>
     </r>
@@ -309,7 +291,137 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Distanciel
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Log. Cours</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">TD Réseaux
+G1/D101</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="7"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Hybride </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">PFA Cours G Amphi</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Log.  TD G1 et
+TD G2
+P. Amphi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TP PFA G4/D104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TD Algo
+G2/D201</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TD Algo
+G1/D203</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TD Algo
+G3/D201</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log.  TD G3/B107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TD GLA G3 D101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TP PFA G7/D103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TP PFA G2/E203, G3/E204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21/09/20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TD GLA G1/D203</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="7"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Présentiel </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Sys.TP G1/E203, G2/E204, G3/E205</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="7"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Distanciel
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Syst. Cours</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="7"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Distanciel </t>
     </r>
@@ -320,14 +432,9 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Log. Cours G Amphi</t>
+      <t xml:space="preserve">Réseau Avan. Cours</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">TD Réseaux
-G1/D101</t>
   </si>
   <si>
     <r>
@@ -337,20 +444,18 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Hybride </t>
+      <t xml:space="preserve">Présentiel  </t>
     </r>
     <r>
       <rPr>
-        <b val="true"/>
         <sz val="7"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">PFA Cours G Amphi</t>
+      <t xml:space="preserve">Sys.TP G4/E201
+G5/E203</t>
     </r>
   </si>
   <si>
@@ -358,44 +463,62 @@
 G1/B107</t>
   </si>
   <si>
-    <t xml:space="preserve">TP PFA G4/D104</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TD Algo
-G2/D201</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TD Algo
-G1/D203</t>
+    <t xml:space="preserve">@[10:00 12:45]TD Réseaux
+G2/E105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TD GLA G2 D203</t>
   </si>
   <si>
     <t xml:space="preserve">Log.  TD
 G2/E107</t>
   </si>
   <si>
-    <t xml:space="preserve">TD Algo
-G3/D201</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Log.  TD G3/B107</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TD GLA G3 D101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TP PFA G7/D103</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TP PFA G2/E203, G3/E204</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21/09/20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TD GLA G1/D203</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sys.TP G1/E203, G2/E204, G3/E205</t>
+    <t xml:space="preserve">@[10:00 12:45]TD Réseaux
+G3/E212</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28/09/20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TP GLA G1/E204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TP GLA G2 E204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TP GLA G3 E201</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05/10/20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TD Réseaux
+G1/E210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12/10/20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TD GLA G3 D201</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19/10/20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESERVE OU PARTIELS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partiel Réseaux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26/10/20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vacances de TOUSSAINT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/11/20</t>
   </si>
   <si>
     <r>
@@ -405,7 +528,28 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Présentiel  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Sys.TP G4/D103
+G5/D104</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="7"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Distanciel </t>
     </r>
@@ -416,75 +560,30 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Réseau Avan. Cours G Amphi</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Sys.TP G4/E201
-G5/E203</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@[10:00 12:45]TD Réseaux
-G2/E105</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TD GLA G2 D203</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@[10:00 12:45]TD Réseaux
-G3/E212</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28/09/20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TP GLA G1/E204</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TP GLA G2 E204</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TP GLA G3 E201</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05/10/20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TD Réseaux
-G1/E210</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12/10/20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TD GLA G3 D201</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19/10/20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESERVE OU PARTIELS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Partiel Réseaux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26/10/20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vacances de TOUSSAINT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02/11/20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sys.TP G4/D103
-G5/D104</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sys.TP G1/E203, G2/E204, G2/E205</t>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="7"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Présentiel </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Sys.TP G1/E203, G2/E204, G2/E205</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Log.  TD
@@ -575,14 +674,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -590,7 +687,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -598,7 +694,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -606,14 +701,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -621,7 +714,6 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -629,42 +721,36 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="7"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="7"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="9.5"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="7"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="21"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="12">
@@ -927,10 +1013,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -948,10 +1038,6 @@
     </xf>
     <xf numFmtId="164" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1073,17 +1159,17 @@
   </sheetPr>
   <dimension ref="A1:AG58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AD8" activeCellId="0" sqref="AD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="0.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="0.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="1.89"/>
@@ -1091,22 +1177,22 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="0.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="0.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="0.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="10.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="0.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="0.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="10.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="1.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="10.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="0.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="0.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="10.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="1.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="10.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="0" width="0.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="0" width="0.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="31" style="0" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="21.78"/>
   </cols>
@@ -1444,7 +1530,7 @@
       <c r="AE7" s="8"/>
       <c r="AF7" s="8"/>
     </row>
-    <row r="8" customFormat="false" ht="19.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2"/>
       <c r="B8" s="10" t="s">
         <v>28</v>
@@ -1456,8 +1542,8 @@
         <v>29</v>
       </c>
       <c r="G8" s="8"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="23"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="14"/>
       <c r="J8" s="15" t="s">
         <v>21</v>
       </c>
@@ -1504,7 +1590,7 @@
       <c r="AE8" s="26"/>
       <c r="AF8" s="8"/>
     </row>
-    <row r="9" customFormat="false" ht="19.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1512,8 +1598,8 @@
       <c r="E9" s="2"/>
       <c r="F9" s="22"/>
       <c r="G9" s="8"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="23"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="14"/>
       <c r="J9" s="15"/>
       <c r="K9" s="8"/>
       <c r="L9" s="16"/>
@@ -1530,9 +1616,7 @@
       <c r="U9" s="19"/>
       <c r="V9" s="8"/>
       <c r="W9" s="20"/>
-      <c r="X9" s="25" t="s">
-        <v>37</v>
-      </c>
+      <c r="X9" s="25"/>
       <c r="Y9" s="22"/>
       <c r="Z9" s="7"/>
       <c r="AA9" s="26"/>
@@ -1549,19 +1633,19 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G10" s="8"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="23"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="14"/>
       <c r="J10" s="15"/>
       <c r="K10" s="8"/>
       <c r="L10" s="16"/>
       <c r="M10" s="23"/>
       <c r="N10" s="7"/>
       <c r="O10" s="17"/>
-      <c r="P10" s="25" t="s">
-        <v>39</v>
+      <c r="P10" s="27" t="s">
+        <v>38</v>
       </c>
       <c r="Q10" s="8"/>
       <c r="R10" s="18"/>
@@ -1570,18 +1654,18 @@
       <c r="U10" s="19"/>
       <c r="V10" s="8"/>
       <c r="W10" s="20"/>
-      <c r="X10" s="27" t="s">
+      <c r="X10" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y10" s="22" t="s">
         <v>40</v>
-      </c>
-      <c r="Y10" s="22" t="s">
-        <v>41</v>
       </c>
       <c r="Z10" s="7"/>
       <c r="AA10" s="8"/>
       <c r="AB10" s="21"/>
       <c r="AC10" s="20"/>
       <c r="AD10" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AE10" s="22"/>
       <c r="AF10" s="8"/>
@@ -1589,29 +1673,29 @@
     <row r="11" customFormat="false" ht="23.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="2"/>
       <c r="B11" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="29"/>
+      <c r="D11" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="29" t="s">
-        <v>44</v>
-      </c>
       <c r="E11" s="12"/>
-      <c r="F11" s="30" t="s">
+      <c r="F11" s="31" t="s">
         <v>29</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="7"/>
-      <c r="I11" s="31" t="s">
+      <c r="I11" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="J11" s="15" t="s">
         <v>45</v>
-      </c>
-      <c r="J11" s="15" t="s">
-        <v>21</v>
       </c>
       <c r="K11" s="8"/>
       <c r="L11" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="M11" s="31" t="s">
+      <c r="M11" s="15" t="s">
         <v>47</v>
       </c>
       <c r="N11" s="7"/>
@@ -1632,8 +1716,8 @@
       </c>
       <c r="V11" s="8"/>
       <c r="W11" s="20"/>
-      <c r="X11" s="25" t="s">
-        <v>33</v>
+      <c r="X11" s="27" t="s">
+        <v>48</v>
       </c>
       <c r="Y11" s="22" t="s">
         <v>34</v>
@@ -1655,19 +1739,19 @@
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="32" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E12" s="33"/>
-      <c r="F12" s="27" t="s">
-        <v>49</v>
+      <c r="F12" s="28" t="s">
+        <v>50</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="7"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
       <c r="K12" s="8"/>
       <c r="L12" s="16"/>
-      <c r="M12" s="31"/>
+      <c r="M12" s="15"/>
       <c r="N12" s="7"/>
       <c r="O12" s="17"/>
       <c r="P12" s="26" t="s">
@@ -1680,8 +1764,8 @@
       <c r="U12" s="19"/>
       <c r="V12" s="8"/>
       <c r="W12" s="20"/>
-      <c r="X12" s="25" t="s">
-        <v>37</v>
+      <c r="X12" s="27" t="s">
+        <v>51</v>
       </c>
       <c r="Y12" s="22"/>
       <c r="Z12" s="7"/>
@@ -1697,21 +1781,21 @@
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="34" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E13" s="33"/>
-      <c r="F13" s="27"/>
+      <c r="F13" s="28"/>
       <c r="G13" s="8"/>
       <c r="H13" s="7"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
       <c r="K13" s="8"/>
       <c r="L13" s="16"/>
-      <c r="M13" s="31"/>
+      <c r="M13" s="15"/>
       <c r="N13" s="7"/>
       <c r="O13" s="17"/>
-      <c r="P13" s="25" t="s">
-        <v>39</v>
+      <c r="P13" s="27" t="s">
+        <v>38</v>
       </c>
       <c r="Q13" s="8"/>
       <c r="R13" s="18"/>
@@ -1720,18 +1804,18 @@
       <c r="U13" s="19"/>
       <c r="V13" s="8"/>
       <c r="W13" s="20"/>
-      <c r="X13" s="27" t="s">
+      <c r="X13" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y13" s="22" t="s">
         <v>40</v>
-      </c>
-      <c r="Y13" s="22" t="s">
-        <v>41</v>
       </c>
       <c r="Z13" s="7"/>
       <c r="AA13" s="8"/>
       <c r="AB13" s="21"/>
       <c r="AC13" s="20"/>
       <c r="AD13" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AE13" s="22"/>
       <c r="AF13" s="8"/>
@@ -1743,15 +1827,15 @@
       <c r="D14" s="34"/>
       <c r="E14" s="33"/>
       <c r="F14" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G14" s="8"/>
       <c r="H14" s="7"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
       <c r="K14" s="8"/>
       <c r="L14" s="16"/>
-      <c r="M14" s="31"/>
+      <c r="M14" s="15"/>
       <c r="N14" s="7"/>
       <c r="O14" s="17"/>
       <c r="P14" s="17"/>
@@ -1762,7 +1846,7 @@
       <c r="U14" s="19"/>
       <c r="V14" s="8"/>
       <c r="W14" s="20"/>
-      <c r="X14" s="27"/>
+      <c r="X14" s="28"/>
       <c r="Y14" s="22"/>
       <c r="Z14" s="7"/>
       <c r="AA14" s="8"/>
@@ -1775,29 +1859,29 @@
     <row r="15" customFormat="false" ht="23.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="2"/>
       <c r="B15" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="C15" s="29"/>
+      <c r="D15" s="30" t="s">
+        <v>54</v>
       </c>
       <c r="E15" s="12"/>
-      <c r="F15" s="30" t="s">
+      <c r="F15" s="31" t="s">
         <v>29</v>
       </c>
       <c r="G15" s="8"/>
       <c r="H15" s="7"/>
-      <c r="I15" s="31" t="s">
+      <c r="I15" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="J15" s="15" t="s">
         <v>45</v>
-      </c>
-      <c r="J15" s="15" t="s">
-        <v>21</v>
       </c>
       <c r="K15" s="8"/>
       <c r="L15" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="M15" s="31" t="s">
+      <c r="M15" s="15" t="s">
         <v>47</v>
       </c>
       <c r="N15" s="7"/>
@@ -1818,8 +1902,8 @@
       </c>
       <c r="V15" s="8"/>
       <c r="W15" s="20"/>
-      <c r="X15" s="25" t="s">
-        <v>33</v>
+      <c r="X15" s="27" t="s">
+        <v>48</v>
       </c>
       <c r="Y15" s="22" t="s">
         <v>34</v>
@@ -1841,19 +1925,19 @@
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="32" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E16" s="33"/>
-      <c r="F16" s="27" t="s">
-        <v>53</v>
+      <c r="F16" s="28" t="s">
+        <v>55</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="7"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
       <c r="K16" s="8"/>
       <c r="L16" s="16"/>
-      <c r="M16" s="31"/>
+      <c r="M16" s="15"/>
       <c r="N16" s="7"/>
       <c r="O16" s="17"/>
       <c r="P16" s="26" t="s">
@@ -1866,8 +1950,8 @@
       <c r="U16" s="19"/>
       <c r="V16" s="8"/>
       <c r="W16" s="20"/>
-      <c r="X16" s="25" t="s">
-        <v>37</v>
+      <c r="X16" s="27" t="s">
+        <v>51</v>
       </c>
       <c r="Y16" s="22"/>
       <c r="Z16" s="7"/>
@@ -1883,21 +1967,21 @@
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="34" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E17" s="33"/>
-      <c r="F17" s="27"/>
+      <c r="F17" s="28"/>
       <c r="G17" s="8"/>
       <c r="H17" s="7"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="31"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
       <c r="K17" s="8"/>
       <c r="L17" s="16"/>
-      <c r="M17" s="31"/>
+      <c r="M17" s="15"/>
       <c r="N17" s="7"/>
       <c r="O17" s="17"/>
-      <c r="P17" s="25" t="s">
-        <v>39</v>
+      <c r="P17" s="27" t="s">
+        <v>38</v>
       </c>
       <c r="Q17" s="8"/>
       <c r="R17" s="18"/>
@@ -1906,18 +1990,18 @@
       <c r="U17" s="19"/>
       <c r="V17" s="8"/>
       <c r="W17" s="20"/>
-      <c r="X17" s="27" t="s">
-        <v>54</v>
+      <c r="X17" s="28" t="s">
+        <v>56</v>
       </c>
       <c r="Y17" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Z17" s="7"/>
       <c r="AA17" s="8"/>
       <c r="AB17" s="21"/>
       <c r="AC17" s="20"/>
       <c r="AD17" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AE17" s="22"/>
       <c r="AF17" s="8"/>
@@ -1929,15 +2013,15 @@
       <c r="D18" s="34"/>
       <c r="E18" s="33"/>
       <c r="F18" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="7"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="31"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
       <c r="K18" s="8"/>
       <c r="L18" s="16"/>
-      <c r="M18" s="31"/>
+      <c r="M18" s="15"/>
       <c r="N18" s="7"/>
       <c r="O18" s="17"/>
       <c r="P18" s="17"/>
@@ -1948,7 +2032,7 @@
       <c r="U18" s="19"/>
       <c r="V18" s="8"/>
       <c r="W18" s="20"/>
-      <c r="X18" s="27"/>
+      <c r="X18" s="28"/>
       <c r="Y18" s="22"/>
       <c r="Z18" s="7"/>
       <c r="AA18" s="8"/>
@@ -1961,27 +2045,27 @@
     <row r="19" customFormat="false" ht="23.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="2"/>
       <c r="B19" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="28"/>
-      <c r="D19" s="29" t="s">
-        <v>44</v>
+        <v>57</v>
+      </c>
+      <c r="C19" s="29"/>
+      <c r="D19" s="30" t="s">
+        <v>43</v>
       </c>
       <c r="E19" s="12"/>
-      <c r="F19" s="30" t="s">
+      <c r="F19" s="31" t="s">
         <v>29</v>
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="7"/>
-      <c r="I19" s="31" t="s">
+      <c r="I19" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="J19" s="15" t="s">
         <v>45</v>
-      </c>
-      <c r="J19" s="15" t="s">
-        <v>21</v>
       </c>
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
-      <c r="M19" s="31" t="s">
+      <c r="M19" s="15" t="s">
         <v>47</v>
       </c>
       <c r="N19" s="7"/>
@@ -1989,7 +2073,7 @@
         <v>30</v>
       </c>
       <c r="P19" s="24" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q19" s="8"/>
       <c r="R19" s="18" t="s">
@@ -2002,8 +2086,8 @@
       </c>
       <c r="V19" s="8"/>
       <c r="W19" s="33"/>
-      <c r="X19" s="25" t="s">
-        <v>33</v>
+      <c r="X19" s="27" t="s">
+        <v>48</v>
       </c>
       <c r="Y19" s="22" t="s">
         <v>34</v>
@@ -2025,19 +2109,19 @@
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="32" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E20" s="33"/>
-      <c r="F20" s="27" t="s">
-        <v>49</v>
+      <c r="F20" s="28" t="s">
+        <v>50</v>
       </c>
       <c r="G20" s="8"/>
       <c r="H20" s="7"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
-      <c r="M20" s="31"/>
+      <c r="M20" s="15"/>
       <c r="N20" s="7"/>
       <c r="O20" s="17"/>
       <c r="P20" s="26" t="s">
@@ -2050,8 +2134,8 @@
       <c r="U20" s="19"/>
       <c r="V20" s="8"/>
       <c r="W20" s="33"/>
-      <c r="X20" s="25" t="s">
-        <v>37</v>
+      <c r="X20" s="27" t="s">
+        <v>51</v>
       </c>
       <c r="Y20" s="22"/>
       <c r="Z20" s="7"/>
@@ -2067,21 +2151,21 @@
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="34" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E21" s="33"/>
-      <c r="F21" s="27"/>
+      <c r="F21" s="28"/>
       <c r="G21" s="8"/>
       <c r="H21" s="7"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="31"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
-      <c r="M21" s="31"/>
+      <c r="M21" s="15"/>
       <c r="N21" s="7"/>
       <c r="O21" s="17"/>
-      <c r="P21" s="25" t="s">
-        <v>39</v>
+      <c r="P21" s="27" t="s">
+        <v>38</v>
       </c>
       <c r="Q21" s="8"/>
       <c r="R21" s="18"/>
@@ -2090,18 +2174,18 @@
       <c r="U21" s="19"/>
       <c r="V21" s="8"/>
       <c r="W21" s="33"/>
-      <c r="X21" s="27" t="s">
+      <c r="X21" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y21" s="22" t="s">
         <v>40</v>
-      </c>
-      <c r="Y21" s="22" t="s">
-        <v>41</v>
       </c>
       <c r="Z21" s="7"/>
       <c r="AA21" s="8"/>
       <c r="AB21" s="21"/>
       <c r="AC21" s="33"/>
       <c r="AD21" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AE21" s="22"/>
       <c r="AF21" s="8"/>
@@ -2113,15 +2197,15 @@
       <c r="D22" s="34"/>
       <c r="E22" s="33"/>
       <c r="F22" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G22" s="8"/>
       <c r="H22" s="7"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="31"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
-      <c r="M22" s="31"/>
+      <c r="M22" s="15"/>
       <c r="N22" s="7"/>
       <c r="O22" s="17"/>
       <c r="P22" s="17"/>
@@ -2132,7 +2216,7 @@
       <c r="U22" s="19"/>
       <c r="V22" s="8"/>
       <c r="W22" s="33"/>
-      <c r="X22" s="27"/>
+      <c r="X22" s="28"/>
       <c r="Y22" s="22"/>
       <c r="Z22" s="7"/>
       <c r="AA22" s="8"/>
@@ -2145,27 +2229,27 @@
     <row r="23" customFormat="false" ht="22.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="2"/>
       <c r="B23" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="29" t="s">
-        <v>44</v>
+        <v>59</v>
+      </c>
+      <c r="C23" s="29"/>
+      <c r="D23" s="30" t="s">
+        <v>43</v>
       </c>
       <c r="E23" s="12"/>
-      <c r="F23" s="30" t="s">
+      <c r="F23" s="31" t="s">
         <v>29</v>
       </c>
       <c r="G23" s="8"/>
       <c r="H23" s="7"/>
-      <c r="I23" s="31" t="s">
+      <c r="I23" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="J23" s="15" t="s">
         <v>45</v>
-      </c>
-      <c r="J23" s="15" t="s">
-        <v>21</v>
       </c>
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
-      <c r="M23" s="31" t="s">
+      <c r="M23" s="15" t="s">
         <v>47</v>
       </c>
       <c r="N23" s="7"/>
@@ -2186,8 +2270,8 @@
       </c>
       <c r="V23" s="8"/>
       <c r="W23" s="8"/>
-      <c r="X23" s="25" t="s">
-        <v>33</v>
+      <c r="X23" s="27" t="s">
+        <v>48</v>
       </c>
       <c r="Y23" s="22" t="s">
         <v>34</v>
@@ -2204,24 +2288,24 @@
       <c r="AE23" s="26"/>
       <c r="AF23" s="8"/>
     </row>
-    <row r="24" customFormat="false" ht="23.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="32" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E24" s="33"/>
-      <c r="F24" s="27" t="s">
-        <v>49</v>
+      <c r="F24" s="28" t="s">
+        <v>50</v>
       </c>
       <c r="G24" s="8"/>
       <c r="H24" s="7"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
-      <c r="M24" s="31"/>
+      <c r="M24" s="15"/>
       <c r="N24" s="7"/>
       <c r="O24" s="17"/>
       <c r="P24" s="26"/>
@@ -2232,8 +2316,8 @@
       <c r="U24" s="19"/>
       <c r="V24" s="8"/>
       <c r="W24" s="8"/>
-      <c r="X24" s="25" t="s">
-        <v>37</v>
+      <c r="X24" s="27" t="s">
+        <v>51</v>
       </c>
       <c r="Y24" s="22"/>
       <c r="Z24" s="7"/>
@@ -2249,21 +2333,21 @@
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="34" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E25" s="33"/>
-      <c r="F25" s="27"/>
+      <c r="F25" s="28"/>
       <c r="G25" s="8"/>
       <c r="H25" s="7"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="31"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
-      <c r="M25" s="31"/>
+      <c r="M25" s="15"/>
       <c r="N25" s="7"/>
       <c r="O25" s="17"/>
-      <c r="P25" s="25" t="s">
-        <v>39</v>
+      <c r="P25" s="27" t="s">
+        <v>38</v>
       </c>
       <c r="Q25" s="8"/>
       <c r="R25" s="18"/>
@@ -2272,18 +2356,18 @@
       <c r="U25" s="19"/>
       <c r="V25" s="8"/>
       <c r="W25" s="8"/>
-      <c r="X25" s="27" t="s">
-        <v>58</v>
+      <c r="X25" s="28" t="s">
+        <v>60</v>
       </c>
       <c r="Y25" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Z25" s="7"/>
       <c r="AA25" s="8"/>
       <c r="AB25" s="21"/>
       <c r="AC25" s="8"/>
       <c r="AD25" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AE25" s="22"/>
       <c r="AF25" s="8"/>
@@ -2295,15 +2379,15 @@
       <c r="D26" s="34"/>
       <c r="E26" s="33"/>
       <c r="F26" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G26" s="8"/>
       <c r="H26" s="7"/>
-      <c r="I26" s="31"/>
-      <c r="J26" s="31"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
-      <c r="M26" s="31"/>
+      <c r="M26" s="15"/>
       <c r="N26" s="7"/>
       <c r="O26" s="17"/>
       <c r="P26" s="17"/>
@@ -2314,7 +2398,7 @@
       <c r="U26" s="19"/>
       <c r="V26" s="8"/>
       <c r="W26" s="8"/>
-      <c r="X26" s="27"/>
+      <c r="X26" s="28"/>
       <c r="Y26" s="22"/>
       <c r="Z26" s="7"/>
       <c r="AA26" s="8"/>
@@ -2327,10 +2411,10 @@
     <row r="27" customFormat="false" ht="17.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="2"/>
       <c r="B27" s="10" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C27" s="35" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D27" s="35"/>
       <c r="E27" s="35"/>
@@ -2341,12 +2425,12 @@
       <c r="J27" s="35"/>
       <c r="K27" s="8"/>
       <c r="L27" s="36" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="M27" s="36"/>
       <c r="N27" s="7"/>
       <c r="O27" s="37" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="P27" s="37"/>
       <c r="Q27" s="37"/>
@@ -2403,10 +2487,10 @@
     <row r="29" customFormat="false" ht="71.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="2"/>
       <c r="B29" s="10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C29" s="38" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D29" s="38"/>
       <c r="E29" s="38"/>
@@ -2441,32 +2525,32 @@
     <row r="30" customFormat="false" ht="23.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="2"/>
       <c r="B30" s="10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C30" s="8"/>
-      <c r="D30" s="27" t="s">
+      <c r="D30" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" s="8"/>
+      <c r="F30" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="H30" s="7"/>
+      <c r="I30" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="E30" s="8"/>
-      <c r="F30" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="G30" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="H30" s="7"/>
-      <c r="I30" s="31" t="s">
+      <c r="J30" s="15" t="s">
         <v>45</v>
-      </c>
-      <c r="J30" s="15" t="s">
-        <v>21</v>
       </c>
       <c r="K30" s="8"/>
       <c r="L30" s="16" t="s">
         <v>46</v>
       </c>
       <c r="M30" s="16" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="N30" s="7"/>
       <c r="O30" s="17" t="s">
@@ -2486,15 +2570,15 @@
       </c>
       <c r="V30" s="8"/>
       <c r="W30" s="8"/>
-      <c r="X30" s="25" t="s">
-        <v>33</v>
+      <c r="X30" s="27" t="s">
+        <v>48</v>
       </c>
       <c r="Y30" s="22" t="s">
         <v>34</v>
       </c>
       <c r="Z30" s="7"/>
-      <c r="AA30" s="31" t="s">
-        <v>66</v>
+      <c r="AA30" s="15" t="s">
+        <v>69</v>
       </c>
       <c r="AB30" s="21" t="s">
         <v>27</v>
@@ -2510,15 +2594,15 @@
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="27"/>
+      <c r="D31" s="28"/>
       <c r="E31" s="8"/>
-      <c r="F31" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="G31" s="31"/>
+      <c r="F31" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="G31" s="15"/>
       <c r="H31" s="7"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
       <c r="K31" s="8"/>
       <c r="L31" s="16"/>
       <c r="M31" s="16"/>
@@ -2534,36 +2618,36 @@
       <c r="U31" s="19"/>
       <c r="V31" s="8"/>
       <c r="W31" s="8"/>
-      <c r="X31" s="25" t="s">
-        <v>67</v>
+      <c r="X31" s="27" t="s">
+        <v>70</v>
       </c>
       <c r="Y31" s="22"/>
       <c r="Z31" s="7"/>
-      <c r="AA31" s="31"/>
+      <c r="AA31" s="15"/>
       <c r="AB31" s="21"/>
       <c r="AC31" s="8"/>
       <c r="AD31" s="26"/>
       <c r="AE31" s="26"/>
       <c r="AF31" s="8"/>
     </row>
-    <row r="32" customFormat="false" ht="19.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="23.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="27"/>
+      <c r="D32" s="28"/>
       <c r="E32" s="8"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="31"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="15"/>
       <c r="H32" s="7"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="31"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
       <c r="K32" s="8"/>
       <c r="L32" s="16"/>
       <c r="M32" s="16"/>
       <c r="N32" s="7"/>
       <c r="O32" s="17"/>
-      <c r="P32" s="25" t="s">
-        <v>39</v>
+      <c r="P32" s="27" t="s">
+        <v>38</v>
       </c>
       <c r="Q32" s="8"/>
       <c r="R32" s="18"/>
@@ -2572,35 +2656,35 @@
       <c r="U32" s="19"/>
       <c r="V32" s="8"/>
       <c r="W32" s="8"/>
-      <c r="X32" s="27" t="s">
-        <v>58</v>
+      <c r="X32" s="28" t="s">
+        <v>60</v>
       </c>
       <c r="Y32" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Z32" s="7"/>
-      <c r="AA32" s="31"/>
+      <c r="AA32" s="15"/>
       <c r="AB32" s="21"/>
       <c r="AC32" s="8"/>
       <c r="AD32" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AE32" s="22"/>
       <c r="AF32" s="8"/>
     </row>
-    <row r="33" customFormat="false" ht="22.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="23.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="27"/>
+      <c r="D33" s="28"/>
       <c r="E33" s="8"/>
       <c r="F33" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="G33" s="31"/>
+        <v>37</v>
+      </c>
+      <c r="G33" s="15"/>
       <c r="H33" s="7"/>
-      <c r="I33" s="31"/>
-      <c r="J33" s="31"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
       <c r="K33" s="8"/>
       <c r="L33" s="16"/>
       <c r="M33" s="16"/>
@@ -2614,10 +2698,10 @@
       <c r="U33" s="19"/>
       <c r="V33" s="8"/>
       <c r="W33" s="8"/>
-      <c r="X33" s="27"/>
+      <c r="X33" s="28"/>
       <c r="Y33" s="22"/>
       <c r="Z33" s="7"/>
-      <c r="AA33" s="31"/>
+      <c r="AA33" s="15"/>
       <c r="AB33" s="21"/>
       <c r="AC33" s="8"/>
       <c r="AD33" s="22"/>
@@ -2627,39 +2711,39 @@
     <row r="34" customFormat="false" ht="22.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="2"/>
       <c r="B34" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="C34" s="28"/>
-      <c r="D34" s="29" t="s">
-        <v>52</v>
+        <v>71</v>
+      </c>
+      <c r="C34" s="29"/>
+      <c r="D34" s="30" t="s">
+        <v>54</v>
       </c>
       <c r="E34" s="12"/>
-      <c r="F34" s="30" t="s">
+      <c r="F34" s="31" t="s">
         <v>29</v>
       </c>
       <c r="G34" s="8"/>
       <c r="H34" s="7"/>
-      <c r="I34" s="31" t="s">
+      <c r="I34" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="J34" s="15" t="s">
         <v>45</v>
-      </c>
-      <c r="J34" s="15" t="s">
-        <v>21</v>
       </c>
       <c r="K34" s="8"/>
       <c r="L34" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="31" t="s">
+      <c r="M34" s="15" t="s">
         <v>47</v>
       </c>
       <c r="N34" s="7"/>
       <c r="O34" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="P34" s="3"/>
       <c r="Q34" s="8"/>
       <c r="R34" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="S34" s="3"/>
       <c r="T34" s="7"/>
@@ -2668,8 +2752,8 @@
       </c>
       <c r="V34" s="8"/>
       <c r="W34" s="8"/>
-      <c r="X34" s="25" t="s">
-        <v>33</v>
+      <c r="X34" s="27" t="s">
+        <v>48</v>
       </c>
       <c r="Y34" s="22" t="s">
         <v>34</v>
@@ -2686,24 +2770,24 @@
       <c r="AE34" s="26"/>
       <c r="AF34" s="8"/>
     </row>
-    <row r="35" customFormat="false" ht="23.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="32" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E35" s="33"/>
-      <c r="F35" s="27" t="s">
-        <v>53</v>
+      <c r="F35" s="28" t="s">
+        <v>55</v>
       </c>
       <c r="G35" s="8"/>
       <c r="H35" s="7"/>
-      <c r="I35" s="31"/>
-      <c r="J35" s="31"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
       <c r="K35" s="8"/>
       <c r="L35" s="16"/>
-      <c r="M35" s="31"/>
+      <c r="M35" s="15"/>
       <c r="N35" s="7"/>
       <c r="O35" s="3"/>
       <c r="P35" s="3"/>
@@ -2714,8 +2798,8 @@
       <c r="U35" s="19"/>
       <c r="V35" s="8"/>
       <c r="W35" s="8"/>
-      <c r="X35" s="25" t="s">
-        <v>67</v>
+      <c r="X35" s="27" t="s">
+        <v>70</v>
       </c>
       <c r="Y35" s="22"/>
       <c r="Z35" s="7"/>
@@ -2731,17 +2815,17 @@
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="34" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E36" s="33"/>
-      <c r="F36" s="27"/>
+      <c r="F36" s="28"/>
       <c r="G36" s="8"/>
       <c r="H36" s="7"/>
-      <c r="I36" s="31"/>
-      <c r="J36" s="31"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
       <c r="K36" s="8"/>
       <c r="L36" s="16"/>
-      <c r="M36" s="31"/>
+      <c r="M36" s="15"/>
       <c r="N36" s="7"/>
       <c r="O36" s="3"/>
       <c r="P36" s="3"/>
@@ -2752,18 +2836,18 @@
       <c r="U36" s="19"/>
       <c r="V36" s="8"/>
       <c r="W36" s="8"/>
-      <c r="X36" s="27" t="s">
-        <v>71</v>
+      <c r="X36" s="28" t="s">
+        <v>74</v>
       </c>
       <c r="Y36" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Z36" s="7"/>
       <c r="AA36" s="8"/>
       <c r="AB36" s="21"/>
       <c r="AC36" s="8"/>
       <c r="AD36" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AE36" s="22"/>
       <c r="AF36" s="8"/>
@@ -2775,15 +2859,15 @@
       <c r="D37" s="34"/>
       <c r="E37" s="33"/>
       <c r="F37" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G37" s="8"/>
       <c r="H37" s="7"/>
-      <c r="I37" s="31"/>
-      <c r="J37" s="31"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
       <c r="K37" s="8"/>
       <c r="L37" s="16"/>
-      <c r="M37" s="31"/>
+      <c r="M37" s="15"/>
       <c r="N37" s="7"/>
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
@@ -2794,7 +2878,7 @@
       <c r="U37" s="19"/>
       <c r="V37" s="8"/>
       <c r="W37" s="8"/>
-      <c r="X37" s="27"/>
+      <c r="X37" s="28"/>
       <c r="Y37" s="22"/>
       <c r="Z37" s="7"/>
       <c r="AA37" s="8"/>
@@ -2807,29 +2891,29 @@
     <row r="38" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="2"/>
       <c r="B38" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C38" s="28"/>
-      <c r="D38" s="29" t="s">
-        <v>44</v>
+        <v>75</v>
+      </c>
+      <c r="C38" s="29"/>
+      <c r="D38" s="30" t="s">
+        <v>43</v>
       </c>
       <c r="E38" s="12"/>
-      <c r="F38" s="30" t="s">
+      <c r="F38" s="31" t="s">
         <v>29</v>
       </c>
       <c r="G38" s="8"/>
       <c r="H38" s="7"/>
-      <c r="I38" s="31" t="s">
+      <c r="I38" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="J38" s="15" t="s">
         <v>45</v>
-      </c>
-      <c r="J38" s="15" t="s">
-        <v>21</v>
       </c>
       <c r="K38" s="8"/>
       <c r="L38" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="M38" s="31" t="s">
+      <c r="M38" s="15" t="s">
         <v>47</v>
       </c>
       <c r="N38" s="7"/>
@@ -2850,8 +2934,8 @@
       </c>
       <c r="V38" s="8"/>
       <c r="W38" s="8"/>
-      <c r="X38" s="25" t="s">
-        <v>33</v>
+      <c r="X38" s="27" t="s">
+        <v>48</v>
       </c>
       <c r="Y38" s="22" t="s">
         <v>34</v>
@@ -2873,19 +2957,19 @@
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="32" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E39" s="33"/>
-      <c r="F39" s="27" t="s">
-        <v>49</v>
+      <c r="F39" s="28" t="s">
+        <v>50</v>
       </c>
       <c r="G39" s="8"/>
       <c r="H39" s="7"/>
-      <c r="I39" s="31"/>
-      <c r="J39" s="31"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="15"/>
       <c r="K39" s="8"/>
       <c r="L39" s="16"/>
-      <c r="M39" s="31"/>
+      <c r="M39" s="15"/>
       <c r="N39" s="7"/>
       <c r="O39" s="17"/>
       <c r="P39" s="26" t="s">
@@ -2898,8 +2982,8 @@
       <c r="U39" s="19"/>
       <c r="V39" s="8"/>
       <c r="W39" s="8"/>
-      <c r="X39" s="25" t="s">
-        <v>67</v>
+      <c r="X39" s="27" t="s">
+        <v>70</v>
       </c>
       <c r="Y39" s="22"/>
       <c r="Z39" s="7"/>
@@ -2915,21 +2999,21 @@
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="34" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E40" s="33"/>
-      <c r="F40" s="27"/>
+      <c r="F40" s="28"/>
       <c r="G40" s="8"/>
       <c r="H40" s="7"/>
-      <c r="I40" s="31"/>
-      <c r="J40" s="31"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="15"/>
       <c r="K40" s="8"/>
       <c r="L40" s="16"/>
-      <c r="M40" s="31"/>
+      <c r="M40" s="15"/>
       <c r="N40" s="7"/>
       <c r="O40" s="17"/>
-      <c r="P40" s="25" t="s">
-        <v>39</v>
+      <c r="P40" s="27" t="s">
+        <v>38</v>
       </c>
       <c r="Q40" s="8"/>
       <c r="R40" s="18"/>
@@ -2938,18 +3022,18 @@
       <c r="U40" s="19"/>
       <c r="V40" s="8"/>
       <c r="W40" s="8"/>
-      <c r="X40" s="27" t="s">
-        <v>58</v>
+      <c r="X40" s="28" t="s">
+        <v>60</v>
       </c>
       <c r="Y40" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Z40" s="7"/>
       <c r="AA40" s="8"/>
       <c r="AB40" s="21"/>
       <c r="AC40" s="8"/>
       <c r="AD40" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AE40" s="22"/>
       <c r="AF40" s="8"/>
@@ -2961,15 +3045,15 @@
       <c r="D41" s="34"/>
       <c r="E41" s="33"/>
       <c r="F41" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G41" s="8"/>
       <c r="H41" s="7"/>
-      <c r="I41" s="31"/>
-      <c r="J41" s="31"/>
+      <c r="I41" s="15"/>
+      <c r="J41" s="15"/>
       <c r="K41" s="8"/>
       <c r="L41" s="16"/>
-      <c r="M41" s="31"/>
+      <c r="M41" s="15"/>
       <c r="N41" s="7"/>
       <c r="O41" s="17"/>
       <c r="P41" s="17"/>
@@ -2980,7 +3064,7 @@
       <c r="U41" s="19"/>
       <c r="V41" s="8"/>
       <c r="W41" s="8"/>
-      <c r="X41" s="27"/>
+      <c r="X41" s="28"/>
       <c r="Y41" s="22"/>
       <c r="Z41" s="7"/>
       <c r="AA41" s="8"/>
@@ -2993,29 +3077,29 @@
     <row r="42" customFormat="false" ht="23.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="2"/>
       <c r="B42" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C42" s="28"/>
-      <c r="D42" s="29" t="s">
-        <v>44</v>
+        <v>76</v>
+      </c>
+      <c r="C42" s="29"/>
+      <c r="D42" s="30" t="s">
+        <v>43</v>
       </c>
       <c r="E42" s="12"/>
-      <c r="F42" s="30" t="s">
+      <c r="F42" s="31" t="s">
         <v>29</v>
       </c>
       <c r="G42" s="8"/>
       <c r="H42" s="7"/>
-      <c r="I42" s="31" t="s">
+      <c r="I42" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="J42" s="15" t="s">
         <v>45</v>
-      </c>
-      <c r="J42" s="15" t="s">
-        <v>21</v>
       </c>
       <c r="K42" s="8"/>
       <c r="L42" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="M42" s="31" t="s">
+      <c r="M42" s="15" t="s">
         <v>47</v>
       </c>
       <c r="N42" s="7"/>
@@ -3036,8 +3120,8 @@
       </c>
       <c r="V42" s="8"/>
       <c r="W42" s="8"/>
-      <c r="X42" s="25" t="s">
-        <v>33</v>
+      <c r="X42" s="27" t="s">
+        <v>48</v>
       </c>
       <c r="Y42" s="22" t="s">
         <v>34</v>
@@ -3059,19 +3143,19 @@
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="32" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E43" s="33"/>
-      <c r="F43" s="27" t="s">
-        <v>49</v>
+      <c r="F43" s="28" t="s">
+        <v>50</v>
       </c>
       <c r="G43" s="8"/>
       <c r="H43" s="7"/>
-      <c r="I43" s="31"/>
-      <c r="J43" s="31"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="15"/>
       <c r="K43" s="8"/>
       <c r="L43" s="16"/>
-      <c r="M43" s="31"/>
+      <c r="M43" s="15"/>
       <c r="N43" s="7"/>
       <c r="O43" s="17"/>
       <c r="P43" s="26" t="s">
@@ -3084,8 +3168,8 @@
       <c r="U43" s="19"/>
       <c r="V43" s="8"/>
       <c r="W43" s="8"/>
-      <c r="X43" s="25" t="s">
-        <v>67</v>
+      <c r="X43" s="27" t="s">
+        <v>70</v>
       </c>
       <c r="Y43" s="22"/>
       <c r="Z43" s="7"/>
@@ -3101,21 +3185,21 @@
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="34" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E44" s="33"/>
-      <c r="F44" s="27"/>
+      <c r="F44" s="28"/>
       <c r="G44" s="8"/>
       <c r="H44" s="7"/>
-      <c r="I44" s="31"/>
-      <c r="J44" s="31"/>
+      <c r="I44" s="15"/>
+      <c r="J44" s="15"/>
       <c r="K44" s="8"/>
       <c r="L44" s="16"/>
-      <c r="M44" s="31"/>
+      <c r="M44" s="15"/>
       <c r="N44" s="7"/>
       <c r="O44" s="17"/>
-      <c r="P44" s="25" t="s">
-        <v>39</v>
+      <c r="P44" s="27" t="s">
+        <v>38</v>
       </c>
       <c r="Q44" s="8"/>
       <c r="R44" s="18"/>
@@ -3124,18 +3208,18 @@
       <c r="U44" s="19"/>
       <c r="V44" s="8"/>
       <c r="W44" s="8"/>
-      <c r="X44" s="27" t="s">
-        <v>58</v>
+      <c r="X44" s="28" t="s">
+        <v>60</v>
       </c>
       <c r="Y44" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Z44" s="7"/>
       <c r="AA44" s="8"/>
       <c r="AB44" s="21"/>
       <c r="AC44" s="8"/>
       <c r="AD44" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AE44" s="22"/>
       <c r="AF44" s="8"/>
@@ -3147,15 +3231,15 @@
       <c r="D45" s="34"/>
       <c r="E45" s="33"/>
       <c r="F45" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G45" s="8"/>
       <c r="H45" s="7"/>
-      <c r="I45" s="31"/>
-      <c r="J45" s="31"/>
+      <c r="I45" s="15"/>
+      <c r="J45" s="15"/>
       <c r="K45" s="8"/>
       <c r="L45" s="16"/>
-      <c r="M45" s="31"/>
+      <c r="M45" s="15"/>
       <c r="N45" s="7"/>
       <c r="O45" s="17"/>
       <c r="P45" s="17"/>
@@ -3166,7 +3250,7 @@
       <c r="U45" s="19"/>
       <c r="V45" s="8"/>
       <c r="W45" s="8"/>
-      <c r="X45" s="27"/>
+      <c r="X45" s="28"/>
       <c r="Y45" s="22"/>
       <c r="Z45" s="7"/>
       <c r="AA45" s="8"/>
@@ -3179,27 +3263,27 @@
     <row r="46" customFormat="false" ht="23.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="2"/>
       <c r="B46" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C46" s="28"/>
-      <c r="D46" s="29" t="s">
-        <v>44</v>
+        <v>77</v>
+      </c>
+      <c r="C46" s="29"/>
+      <c r="D46" s="30" t="s">
+        <v>43</v>
       </c>
       <c r="E46" s="12"/>
-      <c r="F46" s="30" t="s">
+      <c r="F46" s="31" t="s">
         <v>29</v>
       </c>
       <c r="G46" s="8"/>
       <c r="H46" s="7"/>
-      <c r="I46" s="31" t="s">
+      <c r="I46" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="J46" s="15" t="s">
         <v>45</v>
-      </c>
-      <c r="J46" s="15" t="s">
-        <v>21</v>
       </c>
       <c r="K46" s="8"/>
       <c r="L46" s="8"/>
-      <c r="M46" s="31" t="s">
+      <c r="M46" s="15" t="s">
         <v>47</v>
       </c>
       <c r="N46" s="7"/>
@@ -3207,7 +3291,7 @@
         <v>30</v>
       </c>
       <c r="P46" s="24" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q46" s="8"/>
       <c r="R46" s="18" t="s">
@@ -3220,8 +3304,8 @@
       </c>
       <c r="V46" s="8"/>
       <c r="W46" s="8"/>
-      <c r="X46" s="25" t="s">
-        <v>33</v>
+      <c r="X46" s="27" t="s">
+        <v>48</v>
       </c>
       <c r="Y46" s="22" t="s">
         <v>34</v>
@@ -3243,19 +3327,19 @@
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="32" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E47" s="33"/>
-      <c r="F47" s="27" t="s">
-        <v>49</v>
+      <c r="F47" s="28" t="s">
+        <v>50</v>
       </c>
       <c r="G47" s="8"/>
       <c r="H47" s="7"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="15"/>
       <c r="K47" s="8"/>
       <c r="L47" s="8"/>
-      <c r="M47" s="31"/>
+      <c r="M47" s="15"/>
       <c r="N47" s="7"/>
       <c r="O47" s="17"/>
       <c r="P47" s="26" t="s">
@@ -3268,8 +3352,8 @@
       <c r="U47" s="19"/>
       <c r="V47" s="8"/>
       <c r="W47" s="8"/>
-      <c r="X47" s="25" t="s">
-        <v>67</v>
+      <c r="X47" s="27" t="s">
+        <v>70</v>
       </c>
       <c r="Y47" s="22"/>
       <c r="Z47" s="7"/>
@@ -3285,21 +3369,21 @@
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="34" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E48" s="33"/>
-      <c r="F48" s="27"/>
+      <c r="F48" s="28"/>
       <c r="G48" s="8"/>
       <c r="H48" s="7"/>
-      <c r="I48" s="31"/>
-      <c r="J48" s="31"/>
+      <c r="I48" s="15"/>
+      <c r="J48" s="15"/>
       <c r="K48" s="8"/>
       <c r="L48" s="8"/>
-      <c r="M48" s="31"/>
+      <c r="M48" s="15"/>
       <c r="N48" s="7"/>
       <c r="O48" s="17"/>
-      <c r="P48" s="25" t="s">
-        <v>39</v>
+      <c r="P48" s="27" t="s">
+        <v>38</v>
       </c>
       <c r="Q48" s="8"/>
       <c r="R48" s="18"/>
@@ -3308,18 +3392,18 @@
       <c r="U48" s="19"/>
       <c r="V48" s="8"/>
       <c r="W48" s="8"/>
-      <c r="X48" s="27" t="s">
-        <v>58</v>
+      <c r="X48" s="28" t="s">
+        <v>60</v>
       </c>
       <c r="Y48" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Z48" s="7"/>
       <c r="AA48" s="8"/>
       <c r="AB48" s="21"/>
       <c r="AC48" s="8"/>
       <c r="AD48" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AE48" s="22"/>
       <c r="AF48" s="8"/>
@@ -3331,15 +3415,15 @@
       <c r="D49" s="34"/>
       <c r="E49" s="33"/>
       <c r="F49" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G49" s="8"/>
       <c r="H49" s="7"/>
-      <c r="I49" s="31"/>
-      <c r="J49" s="31"/>
+      <c r="I49" s="15"/>
+      <c r="J49" s="15"/>
       <c r="K49" s="8"/>
       <c r="L49" s="8"/>
-      <c r="M49" s="31"/>
+      <c r="M49" s="15"/>
       <c r="N49" s="7"/>
       <c r="O49" s="17"/>
       <c r="P49" s="17"/>
@@ -3350,7 +3434,7 @@
       <c r="U49" s="19"/>
       <c r="V49" s="8"/>
       <c r="W49" s="8"/>
-      <c r="X49" s="27"/>
+      <c r="X49" s="28"/>
       <c r="Y49" s="22"/>
       <c r="Z49" s="7"/>
       <c r="AA49" s="8"/>
@@ -3363,27 +3447,27 @@
     <row r="50" customFormat="false" ht="23.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="2"/>
       <c r="B50" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C50" s="28"/>
-      <c r="D50" s="29" t="s">
-        <v>52</v>
+        <v>78</v>
+      </c>
+      <c r="C50" s="29"/>
+      <c r="D50" s="30" t="s">
+        <v>54</v>
       </c>
       <c r="E50" s="12"/>
-      <c r="F50" s="30" t="s">
+      <c r="F50" s="31" t="s">
         <v>29</v>
       </c>
       <c r="G50" s="8"/>
       <c r="H50" s="7"/>
-      <c r="I50" s="31" t="s">
+      <c r="I50" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="J50" s="15" t="s">
         <v>45</v>
-      </c>
-      <c r="J50" s="15" t="s">
-        <v>21</v>
       </c>
       <c r="K50" s="8"/>
       <c r="L50" s="8"/>
-      <c r="M50" s="31" t="s">
+      <c r="M50" s="15" t="s">
         <v>47</v>
       </c>
       <c r="N50" s="7"/>
@@ -3391,7 +3475,7 @@
         <v>30</v>
       </c>
       <c r="P50" s="24" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q50" s="8"/>
       <c r="R50" s="18" t="s">
@@ -3404,8 +3488,8 @@
       </c>
       <c r="V50" s="8"/>
       <c r="W50" s="8"/>
-      <c r="X50" s="25" t="s">
-        <v>33</v>
+      <c r="X50" s="27" t="s">
+        <v>48</v>
       </c>
       <c r="Y50" s="22" t="s">
         <v>34</v>
@@ -3427,19 +3511,19 @@
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="32" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E51" s="33"/>
-      <c r="F51" s="27" t="s">
-        <v>53</v>
+      <c r="F51" s="28" t="s">
+        <v>55</v>
       </c>
       <c r="G51" s="8"/>
       <c r="H51" s="7"/>
-      <c r="I51" s="31"/>
-      <c r="J51" s="31"/>
+      <c r="I51" s="15"/>
+      <c r="J51" s="15"/>
       <c r="K51" s="8"/>
       <c r="L51" s="8"/>
-      <c r="M51" s="31"/>
+      <c r="M51" s="15"/>
       <c r="N51" s="7"/>
       <c r="O51" s="17"/>
       <c r="P51" s="26" t="s">
@@ -3452,8 +3536,8 @@
       <c r="U51" s="19"/>
       <c r="V51" s="8"/>
       <c r="W51" s="8"/>
-      <c r="X51" s="25" t="s">
-        <v>67</v>
+      <c r="X51" s="27" t="s">
+        <v>70</v>
       </c>
       <c r="Y51" s="22"/>
       <c r="Z51" s="7"/>
@@ -3469,21 +3553,21 @@
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="34" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E52" s="33"/>
-      <c r="F52" s="27"/>
+      <c r="F52" s="28"/>
       <c r="G52" s="8"/>
       <c r="H52" s="7"/>
-      <c r="I52" s="31"/>
-      <c r="J52" s="31"/>
+      <c r="I52" s="15"/>
+      <c r="J52" s="15"/>
       <c r="K52" s="8"/>
       <c r="L52" s="8"/>
-      <c r="M52" s="31"/>
+      <c r="M52" s="15"/>
       <c r="N52" s="7"/>
       <c r="O52" s="17"/>
-      <c r="P52" s="25" t="s">
-        <v>39</v>
+      <c r="P52" s="27" t="s">
+        <v>38</v>
       </c>
       <c r="Q52" s="8"/>
       <c r="R52" s="18"/>
@@ -3492,18 +3576,18 @@
       <c r="U52" s="19"/>
       <c r="V52" s="8"/>
       <c r="W52" s="8"/>
-      <c r="X52" s="27" t="s">
-        <v>71</v>
+      <c r="X52" s="28" t="s">
+        <v>74</v>
       </c>
       <c r="Y52" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Z52" s="7"/>
       <c r="AA52" s="8"/>
       <c r="AB52" s="21"/>
       <c r="AC52" s="8"/>
       <c r="AD52" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AE52" s="22"/>
       <c r="AF52" s="8"/>
@@ -3515,15 +3599,15 @@
       <c r="D53" s="34"/>
       <c r="E53" s="33"/>
       <c r="F53" s="26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G53" s="8"/>
       <c r="H53" s="7"/>
-      <c r="I53" s="31"/>
-      <c r="J53" s="31"/>
+      <c r="I53" s="15"/>
+      <c r="J53" s="15"/>
       <c r="K53" s="8"/>
       <c r="L53" s="8"/>
-      <c r="M53" s="31"/>
+      <c r="M53" s="15"/>
       <c r="N53" s="7"/>
       <c r="O53" s="17"/>
       <c r="P53" s="17"/>
@@ -3534,7 +3618,7 @@
       <c r="U53" s="19"/>
       <c r="V53" s="8"/>
       <c r="W53" s="8"/>
-      <c r="X53" s="27"/>
+      <c r="X53" s="28"/>
       <c r="Y53" s="22"/>
       <c r="Z53" s="7"/>
       <c r="AA53" s="8"/>
@@ -3547,10 +3631,10 @@
     <row r="54" customFormat="false" ht="35.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="2"/>
       <c r="B54" s="10" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C54" s="37" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D54" s="37"/>
       <c r="E54" s="37"/>
@@ -3561,12 +3645,12 @@
       <c r="J54" s="37"/>
       <c r="K54" s="8"/>
       <c r="L54" s="36" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="M54" s="36"/>
       <c r="N54" s="7"/>
       <c r="O54" s="37" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="P54" s="37"/>
       <c r="Q54" s="37"/>
@@ -3589,10 +3673,10 @@
     <row r="55" customFormat="false" ht="35.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="2"/>
       <c r="B55" s="10" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C55" s="38" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D55" s="38"/>
       <c r="E55" s="38"/>
@@ -3627,7 +3711,7 @@
     <row r="56" customFormat="false" ht="35.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="2"/>
       <c r="B56" s="10" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C56" s="38"/>
       <c r="D56" s="38"/>
@@ -3662,7 +3746,7 @@
     </row>
     <row r="57" customFormat="false" ht="19.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="39" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B57" s="39"/>
       <c r="C57" s="39"/>
@@ -3694,7 +3778,7 @@
       <c r="AC57" s="39"/>
       <c r="AD57" s="39"/>
       <c r="AE57" s="40" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="AF57" s="40"/>
       <c r="AG57" s="40"/>
@@ -3803,9 +3887,9 @@
     <mergeCell ref="U8:U10"/>
     <mergeCell ref="V8:V10"/>
     <mergeCell ref="W8:W10"/>
+    <mergeCell ref="X8:X9"/>
     <mergeCell ref="Y8:Y9"/>
     <mergeCell ref="AA8:AA9"/>
-    <mergeCell ref="AB8:AB10"/>
     <mergeCell ref="AC8:AC10"/>
     <mergeCell ref="AD8:AE9"/>
     <mergeCell ref="AF8:AF10"/>

</xml_diff>